<commit_message>
updates to main, added logger
</commit_message>
<xml_diff>
--- a/aiswre/data/incose_guide_sections_df.xlsx
+++ b/aiswre/data/incose_guide_sections_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="262">
   <si>
     <t>start</t>
   </si>
@@ -44,18 +44,6 @@
   </si>
   <si>
     <t>examples</t>
-  </si>
-  <si>
-    <t>system_base_message</t>
-  </si>
-  <si>
-    <t>user_base_message</t>
-  </si>
-  <si>
-    <t>system_message</t>
-  </si>
-  <si>
-    <t>user_message</t>
   </si>
   <si>
     <t>4.1.1</t>
@@ -5043,1407 +5031,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 
-For sets of needs or requirements, an outline can be defined that organizes them in categories or 
-by type.   
-Examples of Type/Category of needs and requirements include:  
-• 
-Function: Functional/Performance. 
-• 
-Fit: Operational: interactions with external systems - input, output, external interfaces, 
-operational environmental, facility, ergonomic, compatibility with existing systems, logistics, 
-users, training, installation, transportation, storage. 
-• 
-Quality (-ilities): reliability, availability, maintainability, accessibility, transportability, quality 
-provisions, growth capacity. 
-• 
-Form: physical characteristics. 
-• 
-Compliance:  
-– 
-Standards and regulations—policy and regulatory. 
-– 
-Constraints—imposed on the project and the project must show compliance. 
-– 
-Business rules—a rule imposed by the enterprise or business unit. 
-– 
-Business requirements—a requirement imposed by the enterprise or business unit. 
-Refer to the NRM Sections 4 and 6 for a more detailed discussion on this approach to organizing 
-needs and requirements. 
-Outlines for organizing needs and requirements can come from international standards or an 
-organizational standard tailored to the organization’s domain and different types of products 
-within that domain.  (The organization for system level needs and requirements may be different 
-than the organization of a set of software needs and requirements.) 
-</t>
-  </si>
-  <si>
-    <t>Step 1 - The user will hand over a Requirement, Criteria, and Examples. Your task is to revise the Requirement as per the provided Criteria and Examples, starting with the phrase "Initial Revision:".
-Step 2 - Compare the initial revision performed in Step 1 against the criteria to determine if any additional revisions are necessary. Let's think step-by-step.
-Step 3 - Return the final requirement revision based on Steps 1 and 2, starting with the phrase "Final Revision:".</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria: {definition}
-Examples: {examples}</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Need statements and requirement statements must conform to one of the agreed patterns, thus 
-resulting in a well-structured complete statement. 
-Examples:  
-See Appendix C, for examples of need statements and requirement statement patterns. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use the active voice in the need statement or requirement statement with the responsible entity 
-clearly identified as the subject of the sentence. 
-Examples:  
-Unacceptable: The Identity of the Customer shall be confirmed.   
-[This is unacceptable because it does not identify the entity that is responsible/accountable for 
-confirming the identity.] 
-Improved by adding the subject: The Identity of the Customer shall be confirmed by the 
-Accounting_System.   
-[Although this statement makes the subject clear, it is still unacceptable because the statement 
-is in the passive voice in that the entity that is responsible/accountable for recording the audio 
-is at the end of the statement rather than the beginning.] 
-Improved: The Accounting_System shall confirm the Customer_Identity. 
-_x000C_Guide to Writing Requirements 
-66 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-[Note that “Accounting_System”, “confirm”, and “Customer_Identity” must be defined in the 
-glossary since there are a number of possible interpretations of these terms—see R4. Also 
-note that this statement is improved because it is in the active voice but, before it is 
-acceptable, it needs to be further improved through the addition of appropriate condition and 
-qualifying clauses]  
-Unacceptable: While in the Operations_Mode, the Audio having the characteristics defined in 
-&lt;ICD xxxx&gt; shall be recorded.   
-[This is unacceptable because the entity that is responsible/accountable for recording the 
-audio is not stated, which makes it difficult to identify which entity is responsible for the action, 
-or how verification is to occur.  In addition, the characteristics of the Audio are not referenced, 
-nor are the conditions under which the action specified.] 
-Improved by adding the subject: While in the Operations_Mode, the Audio having the 
-characteristics defined in &lt;ICD xxxx&gt; shall be recorded by the &lt;SOI&gt;.   
-[Although this statement makes the subject clear, it is still unacceptable because the statement 
-is in the passive voice in that the entity that is responsible/accountable for recording the audio 
-is at the end of the statement rather than the beginning.] 
-Improved: While in the Operations_Mode, the &lt;SOI&gt; shall record Audio having the characteristics 
-defined in &lt;ICD xxxx&gt;.   
-[This is improved because it is in the active voice, but appropriate performance parameters 
-should be added before the statement is acceptable. Also note that “Audio” must be defined in 
-the glossary or data dictionary and required performance added for the requirement to be 
-complete. The characteristics of the Audio received from a &lt;xxxx&gt; source is defined in the 
-ICD.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Ensure the subject and verb of the need or requirement statement are appropriate to the entity to 
-which the statement refers. 
-Examples:  
-Subject examples: 
-Business management requirements have the form “The &lt;business&gt; shall …”.  For example, 
-“ACME_Transport shall …”. 
-Business operations requirements on business elements have the form “The &lt;business element&gt; 
-shall …”. For example, requirements on personnel roles have the form: “The &lt;personnel role&gt; 
-shall …”—such as, “The Production_Manager shall …”; “The Marketing_Manager shall …”. 
-System level needs have the form “The &lt;stakeholders&gt; need the system to ……” 
-System requirements have the form "The &lt;SOI&gt; shall ..."—for example, “The Aircraft shall …” 
-Subsystem level needs have the form “The &lt;stakeholders&gt; need the &lt;subsystem&gt; to ……” 
-Subsystem requirements have the form “The &lt;subsystem&gt; shall …" - for example, once the 
-subsystems are defined: “The Engine shall …”; and “The Landing_Gear shall …”. 
-Verb examples: 
-System level stakeholder need: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to process data received 
-from &lt;other system&gt;.” 
-System level requirement: “The &lt;SOI&gt; shall [process] data received from &lt;another system&gt;. 
-having the characteristics defined in &lt;Interface Definition XYZ.&gt;” 
-Through analysis, the verb/function “process” could be decomposed into sub functions such as 
-“receive”, “store”, “calculate”, “report”, and “display”.   
-Then a decision needs to be made regarding the specific subsystem or system element in which 
-these sub functions are to be performed.   
-If more than one subsystem or system element has a role in performing any one of the sub 
-functions, that requirement should be communicated at the system level and allocated to the 
-applicable subsystems or system elements.   
-If a sub function is to be implemented by a single subsystem or system element, then the sub 
-function requirement should be communicated at the subsystem or system element set of 
-requirements and traced back to the higher-level requirement from which it was decomposed. 
-Unacceptable system requirement: “The User shall ...”  
-[As discussed in Section 1.8, this is unacceptable because the requirement should be on the 
-system, not the user or operator of the system.  This wording is often the result of writing 
-requirements directly from user stories or resulting need statements, without doing the 
-_x000C_Guide to Writing Requirements 
-69 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-transformation of the use case or need into a requirement.  Ask, what does the system have to 
-do so that the need can be achieved?] 
-Improved: “The &lt;SOI&gt; shall …”. 
-Unacceptable: The &lt;SOI&gt; shall display the Current_Time on the &lt;Display Device&gt; per &lt;Display 
-Standard xyz&gt;.   
-[Again, “Current_Time” and “Display_Device” must be defined in the glossary or data 
-dictionary. This statement is most likely unacceptable because the Display_Device is either a 
-system element which is presumably at a level lower than the SOI (and is therefore not 
-appropriate to this level), or the Display_Device is a system or system element outside the SOI 
-(and therefore should be handled as an interface since requirements cannot be placed on it by 
-this requirement set). The display standard would be developed by the organization that would 
-define standards to be used when displaying all information by all applications the organization 
-develops including fonts, font sizes, colors, spacing, brightness, human factors, etc.] 
-Improved: The &lt;SOI&gt; shall display the Current_Time per &lt;Display Standard xyz&gt;.   
-[This is improved because the action is appropriate to the level of the requirement set. Note 
-that, before being an acceptable statement, appropriate condition and qualifying clauses must 
-be added.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Define all terms used within the need statement and requirement statement within an associated 
-glossary and/or data dictionary. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall display the current time as defined in &lt;Display Standard xyz&gt;.   
-[This is unacceptable because it is ambiguous. What is “current”? In which time zone? To what 
-degree of accuracy? In which format?] 
-Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;Display Standard xyz&gt;.   
-[Note that “Current_Time” must then be defined in the glossary or data dictionary in terms of 
-accuracy, format, time zone, and units. Further, appropriate condition and qualifying clauses 
-must be included before the statement is acceptable.  In addition, the organization can define a 
-display standard that applies to all products developed by the organizations concerning how 
-information is to be displayed (fonts, colors, size, spacing, human factors, etc.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use the definite article “the” rather than the indefinite article “a”. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall provide a time display.   
-[This is unacceptable for a requirement because it is ambiguous—is the intent to provide a 
-device to display the time or to display the time? If a device to display the time, then this is not 
-appropriate to level.  If to display a time - will any time displayed do?  Is a one-off display of the 
-time satisfactory?  The writer's intention was most likely that they wanted the system to display 
-continuously the current time in a format that is readable, yet if the developer provided a 
-constant display of “10:00 am” (or even a one-off display of any time), they could argue (albeit 
-unreasonably) that they have met the requirement; yet they would have clearly failed to meet 
-the customer's need and intent. 
-Note that, as a need statement: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to display the time.”, the 
-statement is arguably acceptable.  However, as part of the transformation process, the 
-requirement writers must remove the ambiguity - resulting in the following requirement 
-statement (amongst others). 
-Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;display standard xyz&gt;.   
-[Note that “Current_Time” must be defined in the glossary or data dictionary since there are a 
-number of possible meanings and formats of the more-general term “current time.” For 
-completeness, condition and qualifying clauses must also be added before the requirement is 
-acceptable. In addition, the organization can define a standard that applies to all products 
-developed by the organizations concerning how information is to be displayed (fonts, colors, 
-size, spacing, human factors, etc.]  
-Exceptions and relationships: 
-The purpose of this rule is to avoid the ambiguity that arises because “a” or “an” is tantamount to 
-saying, “any one of”.  In some cases, however, the use of an indefinite article is not misleading.  
-For instance, “… with an accuracy of less than 1 second” allows the phrase to read more 
-naturally and there is no ambiguity because of the accuracy quoted. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-When stating quantities, all numbers should have appropriate and consistent units of measure 
-explicitly stated using a common measurement system in terms of the thing the number refers. 
-_x000C_Guide to Writing Requirements 
-72 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Examples:  
-Unacceptable: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 
-degrees.   
-[This is unacceptable because the units used are stated without indicating the specific 
-measurement system used.] 
-Improved: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 degrees 
-Celsius. 
-Unacceptable: The &lt;SOI&gt; shall establish communications as defined in &lt;ICD xyz&gt; with at least 4 
-in less than or equal to 10 seconds.   
-[This is unacceptable because the units used are incomplete.  “4” of what?] 
-Improved: The &lt;SOI&gt; shall &lt;establish communications&gt; as defined in &lt;ICD xyz&gt; with at least 4 
-satellites in less than or equal to 10 seconds  
-_x000C_Guide to Writing Requirements 
-73 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-[Note that the phrase “establish communications” is probably acceptable at the business level 
-when used in a need statement, but the phrase would need further elaboration at lower levels so 
-that the need is decomposed into verifiable requirements relating to frequency, type of 
-communications (voice? data?), quality, bandwidth, etc. which would typically be defined in an 
-ICD that defines the characteristics of the communication signal to be established.] 
-Unacceptable:  
-“The Fuel_System shall have a maximum fuel volume of 60 l”.   
-“When the Fuel_System detects the Fuel_Tank volume is less than 500 ml, the Fuel_System shall 
-notify the operator within 1 second.” 
-[This is unacceptable because the two requirements use different units of measure (“l” and “ml”). 
-Improved:  
-“The Fuel_System shall have a maximum Fuel_Tank volume of 60 l “.   
-“When the Fuel_System detects the Fuel_Tank volume is less than 0.5 l, the Fuel_System shall 
-notify the operator within 1 second.” 
-[Now both requirements are written using the same units of measure(liters).] 
-Additional Acceptable: "The Fuel_System shall have a maximum Fuel_Tank volume of 60 l.” “When 
-the Signal_System detects the Fuel_Tank volume is less than 50 ml, the Signal_System shall light 
-the Low-Fuel_Iindicator within 1 second." 
-[In this particular case, while the property (“Fuel_Tank volume”) remains the same, the 
-component/element is different ("Fuel_System" vs "Signal_System"). The measurement unit can 
-vary because we are dealing with different component–property pairs.] 
-[Note that “Fuel_System” and “Fuel_Tank” must be defined in the glossary or data dictionary.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the use of vague terms. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall usually be online.   
-[This is unacceptable because “usually” is ambiguous - is availability what is meant?] 
-Improved: The &lt;SOI&gt; shall have an Availability of greater than xx% over a period of greater than 
-yyyy hours.   
-[Note that “Availability” must be defined in the glossary or data dictionary since there are a 
-number of possible ways of calculating that measure.  Alternately, the availability could be 
-expressed as a need.  Then the organization responsible for transforming the need into a 
-requirement could develop feasible concepts for meeting the needed availability and derived 
-one or more well-formed requirements that result in the need being met.] 
-Unacceptable: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the 
-Tracking_Information for relevant aircraft within &lt;xxxx seconds&gt; of detection. 
-[This is unacceptable because it does not make explicit which aircraft are relevant.  Additionally, 
-the statement allows the developer to decide what is relevant; such decisions are in the 
-province of the customer, who should make the requirement explicit.] 
-Improved: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the 
-Tracking_Information of each Aircraft located less than or equal to 20 kilometers from the Airfield 
-when in the Operations_Mode within &lt;xxxx seconds&gt; of detection.   
-[Now it is clear for which aircraft the information needs to be displayed.  Note that “Aircraft”, 
-“Tracking_Information”, “Airfield”, and “Operations_Mode” must be defined in the glossary or 
-data dictionary.] 
-Exceptions and relationships: 
-R3 points out that the use of a verb such as “safe”, may be acceptable at the business 
-management or operations level as long as it is unambiguous at that level, decomposed at the 
-lower levels, and is verifiable at the level stated.  Similarly, some vague adjectives may be 
-allowable at the business management or operations level, providing they are not ambiguous at 
-that level. NLP/AI tools providing automatic assessment of this rule shall be flexible enough and 
-tailorable in order not to identify this issue as an error at a business level, while enforcing the 
-absence of vague terms in other lower-level documents. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the inclusion of escape clauses that state vague conditions or possibilities, such as “so far as is 
-possible”, “as little as possible”, “where possible”, “as much as possible”, “if it should prove 
-necessary”, “if necessary”, “to the extent necessary”, “as appropriate”, “as required”, “to the extent 
-practical”, and “if practicable”. 
-Examples:  
-Unacceptable: The GPS shall, where there is sufficient space, display the User_Location in 
-accordance with &lt;Display Standard xyz&gt;.   
-[This is unacceptable because whether there is sufficient space is vague, ambiguous, and 
-unverifiable.  The requirement is clearer without the escape clause.]  
-Improved: The GPS shall display the User_Location in accordance with &lt;Display Standard XYZ&gt;. 
-[Note that appropriate performance measures must also be specified such as within what time, 
-format, and accuracy.  Also note that “GPS” and “User_Location” must be defined in the 
-glossary or data dictionary.]   
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid open-ended, non-specific clauses such as “including but not limited to”, “etc.” and “and so 
-on”. 
-Examples:  
-Unacceptable: The ATM shall display the Customer Account_Number, Account_Balance, and so 
-on per &lt;Display Standard xyz&gt;.   
-[This is unacceptable because it contains an opened list of what is to be displayed.] 
-_x000C_Guide to Writing Requirements 
-76 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Improved: [Split into as many requirements as necessary to be complete.  Note that the types of 
-customer information to be displayed needs to be defined in the glossary.]: 
-The ATM shall display the Customer Account_Number in accordance with &lt;Display Standard 
-xyz&gt;. 
-The ATM shall display the Customer Account_Balance in accordance with &lt;Display Standard 
-xyz&gt;. 
-The ATM shall display the Customer Account_Type in accordance with &lt;Display Standard 
-xyz&gt;. 
-The ATM shall display the Customer Account_Overdraft_Limit in accordance with &lt;Display 
-Standard xyz&gt;. 
-[Note: Some may feel that a bulleted list or table is acceptable.  While, from a readability 
-perspective, this may be true, from a requirement management perspective, each item in the 
-bulleted list is still a requirement.  Because of this requirement statements as in the example 
-above should be written as individual statements especially when allocation, traceability, 
-verification, and validation activities are specific to the single item.  See also R17, R18, R22, 
-and R28.] 
-[Note the above examples are incomplete in that expected performance and under what 
-conditions has not been included in the requirement statements.] 
-4.2 Concision 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the use of superfluous infinitives such as “to be designed to”, “to be able to”, “to be capable 
-of”, “to enable”, “to allow”. 
-Examples:  
-Unacceptable: The Weapon_System shall be able to store the location of each Ordnance.   
-[This is unacceptable because it contains the superfluous infinitive “be able to” which implies the 
-requirement is ubiquitous in that it can be applied at any time, but it therefore begs the question 
-as to the condition under which the feature can be invoked.  However, this is acceptable for the 
-stakeholder need: “The stakeholders need the Weapon_System to be able to store the location 
-of each Ordnance.”] 
-Improved: When &lt;condition&gt;he Weapon_System shall store the Location of each Ordnance.   
-[This is better because the requirement applies only in a particular condition. Note that the 
-terms “Weapon_System”, “Location”, and “Ordnance” must be defined in the glossary or data 
-dictionary. To be complete the appropriate performance characteristics would also need to be 
-defined and included within the requirement statement.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use a separate clause for each condition or qualification. 
-Examples:  
-Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the 
-characteristics defined in &lt;ICD xyz&gt; at an accuracy of less than or equal to 20 meters to each 
-Maritime_User during Harbor_Harbor_Approach_Maneuvering (HHAM).   
-[This is unacceptable because it inserts a phrase in such a way that the object of the sentence 
-is separated from the verb.] 
-Improved: The Navigation_Beacon shall provide Augmentation_Data having the characteristics 
-defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering 
-(HHAM), at an accuracy of less than or equal to 20 meters.   
-[This rewrite places the basic function in an unbroken clause followed by the sub-clause 
-describing performance.  Note that: “Navigation_Beacon”, “Maritime_User”, and 
-“Harbor_Harbor_Approach_Maneuvering (HHAM)” must be defined in the glossary or data 
-dictionary. There is also an issue in that when discussing accuracy, precision needs to also be 
-addressed.] 
-4.3 Non-ambiguity 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use correct grammar. 
-Examples:  
-Unacceptable: The Weapon_System shall storing the location of all ordnance.   
-[This is unacceptable because the grammatical error leads to uncertainty about the meaning.] 
-Improved: The Weapon_System shall store the location of all Ordnance.   
-[Note that “Ordnance” must be defined in the glossary to be explicit about the types of weapons 
-and ammunition. Also, where the location is to be stored and the format of the data, must be 
-addressed. The action “store” needs to be further evaluated to determine if that is an 
-appropriate action (verb) for the Weapon_System vs a user interacting with the 
-Weapon_System as discussed in R3.  Additionally, to be complete any specific performance 
-measures and conditions should be included within the requirement statement.] 
-Unacceptable: When in the Active_State, the Record_Subsystem shall display each of the 
-Names of the Line_Items, without obscuring the User_ID per &lt;Display Standard xyz&gt;. 
-[This is unacceptable because the grammatical error involving the inappropriate placement of 
-“each of”—it is most likely that a Line_Item has only one name.] 
-Improved: When in the Active_State, the Record_Subsystem shall display on &lt;Display Device&gt; 
-the Name of each Line_Item, without obscuring the User_ID per &lt;Display Standard XYZ.&gt;.  
-[This is acceptable the ambiguity has been addressed.  The requirement is now more complete 
-in that it references where the information is to be display and the standard to be used 
-concerning the display of the information. If there are any performance measures that apply, 
-they would also need to be addressed.] 
-Unacceptable: The &lt;corporate website&gt; shall only use Approved_Fonts. 
-[This is unacceptable because it mandates that the website shall only use the designated 
-fonts—that is, it is not expected to perform any other function except to use those fonts. This is 
-clearly not what is meant but becomes ambiguous by the inappropriate grammar and the 
-incorrect placement of the word “only”. What is most likely meant is that the only fonts to be 
-used are the approved fonts defined in the organization’s display standard.] 
-Improved: The &lt;corporate website&gt; shall display information using Approved_Fonts defined in 
-&lt;Display Standard xyz&gt;. 
-_x000C_Guide to Writing Requirements 
-80 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-[This is better because the ambiguity has been addressed.  To be acceptable, any conditions 
-and qualifying clauses would also need to be added.  If the organization has a standard for 
-displaying information that addresses acceptable fonts, font sizes, colors, spacing, human 
-factors, etc., the requirement should refer to that standard.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use correct spelling. 
-Examples:  
-Unacceptable: The Weapon_System shall store the location of each ordinance.   
-[This is unacceptable because the word “ordinance” means regulation or law.  It is unlikely that 
-the Weapon_System is interested in the location of ordinance (regulations).  In the context of a 
-_x000C_Guide to Writing Requirements 
-81 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-weapon system, what the authors meant to use is "ordnance" as in weapons and ammunition, 
-not “ordinance”.] 
-Improved: The Weapon_System shall store the Location of each Ordnance.   
-[Note that “Location” and “Ordnance” must be defined in the glossary or data dictionary to be 
-explicit about the types of weapons and ammunition.  The action “store” needs to be further 
-evaluated to determine if that is an appropriate action (verb) for the Weapon_System vs a user 
-interacting with the Weapon_System as discussed in R3.  Additionally, to be complete any 
-specific performance measures and conditions should be included within the requirement 
-statement.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use correct punctuation. 
-Examples:  
-Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the 
-characteristics defined in &lt;ICD xyz&gt; to each Maritime_User, engaged in 
-Harbor_Harbor_Approach_Maneuvering (HHA) at an accuracy of less than 20 meters.   
-[This is unacceptable because the incorrectly placed comma in this sentence confuses the 
-meaning, leading the reader to believe that the accuracy is related to the maneuver rather than 
-to the augmentation data.]  
-Improved: The Navigation_Beacon shall provide Navigation_Data having the characteristics 
-defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering 
-(HHA), at an accuracy of less than 20 meters. 
-[The positioning of the comma now makes it clear that the accuracy and availability relate to the 
-data. Also note that, while performance measures are included, the appropriate conditions are 
-not addressed.  Further “Navigation_Beacon”, “Navigation_Data”, “Maritime_User”, and 
-“Harbor_Harbor_Approach_Maneuvering (HHA)” must be defined in the glossary or data 
-dictionary.]  
-_x000C_Guide to Writing Requirements 
-82 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use a defined convention to express logical expressions such as “[X AND Y]”, “[X OR Y]”,  
-[X XOR Y]”, “NOT [X OR Y]”. 
-Examples:  
-Unacceptable: The Engine_Management_System shall disengage the 
-Speed_Control_Subsystem within &lt;TBD seconds&gt; when the Cruise_Control is engaged, and the 
-Driver applies the Accelerator.   
-[This is unacceptable because of the ambiguity of “and” could be confused with combining two 
-separate thoughts.  Instead use the form of a logical expression [X AND Y].] 
-Improved: When [the Cruise_Control is Engaged] AND [the Accelerator is Applied], the 
-Engine_Management_System shall Disengage the Speed_Control_Subsystem within &lt;TBD 
-seconds&gt;.  
-[“Engine_Management_System”, “Speed_Control_Subsystem”, “Disengage”, “Engaged”, 
-“Accelerator”, “Applied”, and “Cruise_Control” must be defined in the glossary or data dictionary.] 
-_x000C_Guide to Writing Requirements 
-83 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Exceptions and relationships: 
-While R21: Avoid Parentheses states that parentheses or brackets are to be avoided within 
-general sentence structure, this rule suggests that brackets may be used as part of a convention to 
-avoid ambiguity when expressing a logical expression.   
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the use of the word “not”. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall not fail.   
-[This is unacceptable because verification of the requirement would require infinite time. The 
-requirement is also infeasible in that, as written, the implication is to never fail, under any 
-conditions.] 
-Improved:  
-The &lt;SOI&gt; shall have an Availability of greater than or equal to 95%.  or  
-The &lt;SOI&gt; shall have a Mean Time Between Failures (MTBF) of xx operating hours. 
-[For quality requirements, it would be more precise in the above were written as need 
-statements.  Then those transforming the quality need statements into requirement statements 
-would define feasible concepts that would result in the needed quality attributes and derive well-
-formed requirements on the &lt;SOI&gt; that would result in those needs to be met.] 
-Unacceptable: The &lt;SOI&gt; shall not contain mercury.   
-[This is unacceptable because verification of the requirement would require the ability to 
-measure the amount of mercury with infinite accuracy and precision.  In addition, the real 
-requirement may not be stated, for example, the real concern may be the use of toxic materials, 
-not just mercury.  If that is the case, it may be best to reference a standard from a governmental 
-agency concerning allowable exposures to a list of common toxic materials.] 
-Improved: The &lt;SOI&gt; shall limit metallic mercury exposure to those coming in contact with the 
-&lt;SOI&gt; to less than or equal 0.025 mg/m3 over a period of 8 hours. 
-Exceptions and relationships: 
-It may be reasonable to include “not” in a requirement when the logical “NOT” is implied—for 
-example when using not [X or Y].  In that case, however, in accordance with R15, it may be better 
-to capitalize the “NOT” to make the logical condition explicit: NOT [X or Y].   
-_x000C_Guide to Writing Requirements 
-84 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-There may be other cases such as “The &lt;SOI&gt; shall not be red in color.”, which is stating a 
-constraint and is verifiable, as long as the range of shades of red is stated (RBG rr,bb,gg range or 
-a “name” of red in some standard).   
-The key consideration is verification.  If the “not” can be unambiguously verified, then its use is 
-acceptable. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the use of the oblique (“/”) symbol. 
-Examples:  
-Unacceptable: The User_Management_System shall Open/Close the User_Account in less than 
-1 second.   
-[This is unacceptable because it is unclear as to what is meant by open/close: open, close, or 
-both?] 
-Improved: (Split into two requirements with an appropriate condition)  
-When &lt;condition&gt;, the User_Management_System shall Open the User_Account in less than 1 
-second. 
-When &lt;condition&gt;, the User_Management_System shall Close the User_Account in less than 1 
-second.  
-Unacceptable: When the Clutch is Disengaged and/or the Brake is Applied, the 
-Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;.   
-[This is unacceptable because of the use of “and/or.” If simultaneity is intended—that is the dual 
-conditions must be met at the same time—write the requirements as a logical AND. If “and” is 
-meant in the sense that the action is to be completed under each of the conditions, split the two 
-thoughts into separate requirements, one for each condition.  If “or” is meant, write the 
-requirement as a logical OR.] 
-Improved: (As one requirement if simultaneity is intended): 
-When [the Clutch is Disengaged] AND [the Brake is Applied], the Engine_Management_System 
-shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. 
-_x000C_Guide to Writing Requirements 
-85 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Improved: (As two requirements if two separate conditions are intended): 
-When the Clutch is Disengaged, the Engine_Management_System shall disengage the 
-Speed_Control_Subsystem within &lt;XYZ ms&gt;. 
-When the Brake is Applied, the Engine_Management_System shall disengage the 
-Speed_Control_Subsystem within &lt;XYZ ms&gt;. 
-Improved: (As one requirement if inclusive OR is intended)  
-When EITHER [the Clutch is Disengaged] OR [the Brake is Applied], the 
-Engine_Management_System shall disengage the Speed_Control_Subsystem. 
-4.4 Singularity 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Write a single sentence that contains a single thought conditioned and qualified by relevant sub-
-clauses. 
-Examples:  
-Unacceptable:  When in the Active_State, the Record_Subsystem shall display the Name of each 
-Line_Item and shall record the Location of each Line_Item, without obscuring the User_ID.   
-[This is unacceptable because the sentence contains two requirements and the qualification 
-only applies to the first requirement, not the second.] 
-Improved: (Split into two separate requirements)  
-When in the Active_State, the Record_Subsystem shall display per &lt;Display Standard XYZ&gt; 
-the Name of each Line_Item, without obscuring the User_ID.  
-When in the Active_ State, the Record_Subsystem shall record the Location of each Line_Item. 
-[Note use of the glossary or data dictionary to define terms.  Any applicable performance 
-measures must be addressed for the requirement to be complete.] 
-Unacceptable: The Control_Subsystem will close the Inlet_Valve until the temperature has 
-reduced to 85 °C, when it will then reopen it in less than 1 second.   
-[This is unacceptable because the sentence contains two event driven requirements.  
-Additionally, the sentence contains two occurrences of the pronoun “it” ambiguously referring to 
-different things (see R26), the term “has reduced” is ambiguous, and the action verb must be 
-”shall”, not “will”. Also, a time constraint is included but it is not clear whether it applies to both 
-actions or only the second action.] 
-Improved: (Split into two requirements each with its own time constraint): 
-If the Water_Temperature in the Boiler increases to greater than 85 °C, the Control_Subsystem 
-shall close the Inlet_Valve in less than 1 second.  
-When the Water_Temperature in the Boiler reduces to less than or equal to 85 °C, the 
-Control_Subsystem shall open the Inlet_Valve in less than 1 second. 
-[Note use of the glossary or data dictionary to define terms.]  
-Unacceptable:  
-In the event of a fire detection, within &lt;xxx ms&gt;: 
-• 
-Security entrances shall be set to Free_Access_Mode. 
-• 
-Fire escape doors shall be unlocked. 
-[This is unacceptable because the condition “in the event of a fire detection” is stated following a 
-list of actions to be taken; each of which the system must be verified against.  Also, note the 
-actions are written in passive voice which violates R2.  Each action needs to be communicated 
-in a separate active voice requirement statement.  For multiple conditions for a single action see 
-R28.] 
-Improved: (Split into two requirements) 
-In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode 
-to ON within &lt;xxx ms&gt;. 
-In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock 
-unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within 
-&lt;xxx ms&gt;. 
-[There is a Fire Detection subsystem responsible for detecting fires and setting the 
-Fire_Detection parameter to “TRUE” which triggers the two actions.   All other subsystems that 
-_x000C_Guide to Writing Requirements 
-87 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” 
-will take the required action as stated in their set of requirements.  All Fire Doors will be 
-monitoring for the Fire_Door_Unlock command and will unlock when the command is 
-received.] 
-Unacceptable: The &lt;corporate website&gt; shall use only approved fonts. The approved fonts are: 
-&lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;. 
-[This is unacceptable because it is non-singular. Rather than splitting into three requirements 
-(which is quite difficult to so whilst conforming to the “only” constraint, the term 
-“Approved_Fonts” can be included in the Glossary, which then states: “Approved_Fonts: 
-&lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;.”] 
-Improved: (using the glossary term “Approved_Fonts”) 
-The &lt;corporate website&gt; shall use only Approved_Fonts.  
-[Alternately, the organization can define a display standard which includes a definition of 
-approved fonts, and the requirement could reference that standard.] 
-Improved: (referring to a standard.) 
-The &lt;corporate website&gt; shall display information in accordance with &lt;Display Standard xyz&gt;. 
-[Note that this also allows better configuration management of the requirements database, 
-particularly if the approved fonts are referred to in a number of requirements—that is, should 
-the approved fonts change or characteristics of the fonts change, the list of approved fonts and 
-characteristics only needs to be updated in the Glossary, rather than in multiple requirements 
-(in which case there is a risk that one or more of the requirements is missed).] 
-[In reality, requirements involving the actions such as “display” are interface requirements 
-given that the information will be provided by something to some display device for display.] 
-[Having the information in the display standard then can be referred to in the set of 
-requirements for that display device. Note that referring to a standard also allows for later 
-specialization, for example different parts of the standard may apply to different display 
-devices.] 
-Exceptions and relationships: 
-Every requirement should have a main clause with a main verb (R1).  However, additional sub-
-clauses with auxiliary verbs or adverbs may be used to qualify the requirement with performance 
-attributes. 
-Such sub-clauses cannot be verified in isolation since they are incomprehensible without the 
-main clause.  Sub-clauses that need to be verified separately from others should be expressed as 
-separate requirements. 
-For example, “The Ambulance_Control_System shall communicate Incident_Details to the Driver” 
-is a complete, comprehensible statement with a single main verb.  An auxiliary clause may be 
-added to provide a qualifying constraint “The Ambulance_Control_System shall communicate 
-Incident_Details to the Driver, while simultaneously maintaining communication with the Caller.”  
-[Note: the verb “communicate” is more appropriate for a need statement.  The resulting Design 
-Input Requirements would address the specific means of communication.] 
-_x000C_Guide to Writing Requirements 
-88 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Similarly, if the requirement is to extinguish and dispose of a match as a single combined action, 
-the requirement must ensure that both are verified the same time and allocated the same. 
-Note that, if performance attributes need to be verified separately, they should be expressed as 
-sub-clauses in separate requirements.   
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid words that join or combine clauses, such as “and”, “or”, “then”, “unless”, “but”, “as well as” 
-“but also”, “however”, “whether”, “meanwhile”, “whereas”, “on the other hand”, or “otherwise”. 
-Examples:  
-Unacceptable: The user shall either be trusted or not trusted.  
-[This is unacceptable for several reasons.  The intention is that a user should be classified in 
-one of two ways, but it is also a passive requirement written on the user rather than on the 
-system (R2) and it is ambiguous: the requirement would still be met if the system took the 
-option of treating all users as trusted.] 
-Improved: The Security_System shall categorize each User as EITHER Trusted OR Not_Trusted. 
-Unacceptable:  The &lt;SOI&gt; shall display the Location and Identity of the Lead_Vehicle. 
-[This is unacceptable because is in fact stating two requirements which may well need to be 
-verified by different verification actions. In addition, the format of the displayed information is not 
-referenced.]  
-Improved: (Express as two requirements) 
-The &lt;SOI&gt; shall display the Location of the Lead_Vehicle per &lt;Display Standard xyx&gt;. 
-The &lt;SOI&gt; shall display the Identity of the Lead_Vehicle per &lt;Display Standard xyx&gt;. 
-Unacceptable:  The &lt;SOI&gt; shall provide an audible or visual alarm having the characteristics 
-defined in &lt;alarm standard xyz&gt;. 
-[This is unacceptable because it is a moot point as to whether the designer can choose which 
-alarm to implement, or (which is probably the intent of the writer) whether both alarms are 
-required, and the operator is alerted by at least one.]  
-Improved: (if the choice is available to the designer) 
-The &lt;SOI&gt; shall provide EITHER an Audible_Alarm OR Visual_Alarm having the 
-characteristics defined in &lt;Alarm Standard xyz&gt;. 
-Improved: (if both alarms are required) 
-_x000C_Guide to Writing Requirements 
-89 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-The &lt;SOI&gt; shall provide an Audible_Alarm having the characteristics defined in &lt;Alarm 
-Standard xyz&gt;. 
-The &lt;SOI&gt; shall provide a Visual_Alarm having the characteristics defined in &lt;Alarm Standard 
-xyz&gt;. 
-[As separate requirements, each can be allocated differently, and the SOI will be verified to 
-meet each. 
-Exceptions and relationships: 
-AND, OR, NOT can be used in need and requirement statements as logical conditions and 
-qualifiers as stated in R15. See also R16 and R17. 
-Combinators such as in “Command_and_Control” can be used in the project data dictionary, 
-ontology or glossary to cover one single function or quality of the system. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid phrases that indicate the “purpose of “, “intent of”, or “reason for” the need statement or 
-requirement statement. 
-Examples:  
-Unacceptable: The Record_Subsystem shall display the Name of each Line_Item so that the 
-Operator can confirm that it is the correct Item.   
-[This is unacceptable because the text “so that the Operator can confirm that it is the correct 
-Item” is rationale.] 
-Improved: The Record_Subsystem shall display the Name of each Line_Item per &lt;Display 
-Standard XYZ&gt;.   
-[The text “so that the Operator can confirm that it is the correct Item” should be included in the 
-rationale attribute.] 
-_x000C_Guide to Writing Requirements 
-90 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Unacceptable: The Operation_Logger shall record each Warning_Message produced by the 
-system.   
-[This is unacceptable because of the superfluous words “produced by the system”.] 
-Improved: The Operation_Logger shall record each Warning_Message within &lt;performance 
-measure&gt;. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid parentheses and brackets containing subordinate text. 
-Examples:  
-Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the 
-boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; 
-[This is unacceptable because of the parenthetical phrase as well as the ambiguous word 
-“usually”.   Note that the parameter Water_Temperature needs to be defined in the glossary in 
-order to be specific] 
-Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall 
-disconnect power from the Boiler within &lt;xxx ms&gt;. 
-[Note: for the above example, if this behavior is the result of a design decision, then the 
-requirement needs to be communicated as a design output.  The design input requirement 
-should focus on why this behavior is needed - for example, prevent the boiler from over 
-pressurizing and exploding. This is a good example of the benefit of asking “Why” for 
-requirements of this type.  The answer is the real design input requirement.   If included in the 
-set of Design Input Requirements, then the “why” should be included in the rationale.] 
-Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall 
-prevent the Boiler from over pressurization. 
-[How this is done is a design decision.} 
-Exceptions and relationships: 
-While this rule states brackets are to be avoided, R15 indicates that brackets may be used as 
-part of a convention for eliminating ambiguous conditions such as logical expressions. In that 
-case, it is useful to settle on a combination to be used—that is, for example, the organization 
-_x000C_Guide to Writing Requirements 
-91 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-template may avoid round brackets “(   )” in any statement and may use square brackets “[...]” in 
-logical expressions. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Enumerate sets explicitly instead of using a group noun to name the set. 
-Examples:  
-Unacceptable: The thermal control system shall manage temperature-related functions.   
-[This is unacceptable because there is ambiguity regarding which functions are to be managed 
-as well as what is meant by “managed”.  The specific functions should be enumerated explicitly 
-in separate requirement statements along with performance expectations and any applicable 
-conditions, triggers, or constraints.] 
-Unacceptable: The thermal control system shall monitor system temperature.   
-This is unacceptable because there is ambiguity regarding the function “monitor”.  Similar to 
-“managed” What are the expectations of the stakeholders – update the display of the system 
-temperature, maintain the temperature within some range, or store the history of the system 
-temperature? The specific subfunctions should be enumerated explicitly in separate 
-requirement statements along with performance expectations and any applicable conditions, 
-triggers, or constraints.] 
-Improved: (three separate requirements):  
-The Thermal_Control_System shall update the display of System_Temperature every 10 +/- 1 
-seconds. 
-The Thermal_Control_System shall maintain the System_Temperature between 95°C and 
-98°C.  
-The Thermal_Control_System shall store the history of System_Temperature.  
-[Note use of the glossary to define terms.] 
-Exceptions and relationships: 
-It is almost always better to enumerate members in a set, but the rule may be softened at the 
-higher levels of abstraction if the resulting requirement is sufficiently unambiguous.  For example, 
-at the business management level the business may state “ACME Consulting shall manage 
-_x000C_Guide to Writing Requirements 
-92 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Human Relations (HR) functions centrally.” or a system-level need statement may state: “The 
-&lt;stakeholders&gt; need the &lt;SOI&gt; to manage HR functions centrally.”  
-Although this raises the question of which HR functions are being referred to, it is not useful to 
-include a long list at these levels of abstractions and it is often not necessary since the statement 
-is sufficiently clear at the level at which it is stated.  The detailed enumeration of functions will be 
-undertaken at the business operations level, and the business management stakeholders should 
-be comfortable that no function will be omitted as a result of not listing it at the business 
-management level.   
-At the system level, need statements may include group nouns to name a set of entities or 
-include a higher-level function that is appropriate to the level of abstraction being communicated 
-within the need statement.  During the transformation of the need statement into requirements, 
-the project team would decompose the need into individual functional/performance requirements 
-as well as define requirements concerning the word “centrally” and would then validate with the 
-stakeholders that the resulting requirements, when realized, would meet the intent of the need 
-statement. 
-Another exemption would be to use the glossary or data dictionary to explicitly elaborate the set. 
-For example. “Account_Information” may be defined in the Glossary to include “Account_Name”, 
-“Account_Number”, and “Account_Balance”. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-When a need or requirement is related to complex behavior, refer to a supporting diagram, model, 
-or ICD. 
-Examples:  
-Unacceptable: The Control_System shall close Valves A AND B within 5 seconds of the 
-temperature exceeding 95 °C AND within 2 seconds of each other.   
-[This is unacceptable because of the confusing set of conditions.  In this case what is meant 
-will be clear if the requirement referred to a diagram for context.] 
-Improved: [Within 5 seconds of the temperature exceeding 95 °C] AND [within 2 seconds of each 
-other as shown in Timing_Diagram_6], the Control_System shall close [Valve A AND Valve B].   
-[Note that this assumes, of course, that the timing diagram itself is not ambiguous.  If it is not 
-possible to remove the ambiguity by using a diagram, it may be better to split the requirement 
-into two.] 
-[Note: for the above example, if this complex behavior is the result of a design decision, then 
-the requirement needs to be communicated as a design output.  The design input requirement 
-should focus on why this behavior is needed.] 
-Interface Example: 
-An interface requirement may refer to the characteristics of the electrical power (current/voltage) 
-being supplied by a system.   
-There can be multiple characteristics that need to be defined such that the systems receiving the 
-power have a clear understanding of the characteristics of the power they are receiving.  In this 
-case it is common for the characteristics to be defined in an ICD which both the provider and 
-receiver of the power can refer to in their Design Input Requirements.  From the provider 
-perspective the provider system will have to be verified that the power provided has all of these 
-characteristics and the receiver will have to verify it can receive and operate on power having 
-these same characteristics.   
-&lt;System 1&gt; shall provide power to &lt;System 2&gt; having the characteristics defined in &lt;ICD xyz&gt;. 
-Table 123&gt;. 
-&lt;System 2&gt; shall receive power from &lt;System 1&gt; having the characteristics defined in &lt;ICD 
-xyz&gt;. Table 123&gt;. 
-&lt;System 2&gt; shall operate on power having the characteristics defined in &lt;ICD xyz&gt;. Table 
-123&gt;. 
-4.5 Completeness 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the use of personal and indefinite pronouns. 
-Examples:  
-Unacceptable: The controller shall send the driver his itinerary for the day. It shall be delivered at 
-least 8 hours prior to his Shift.  
-[This is unacceptable because the requirement is expressed as two sentences and the second 
-sentence uses the pronouns “it” and “his.”] 
-Improved: At least 8 hours prior to the Driver_Shift, the Controller shall send the Driver_Itinerary 
-for the day to the Driver.   
-[Note use of the glossary to define terms and to be explicit about the relationship between the 
-driver, shift, and the itinerary for that particular driver.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid relying on headings to support explanation or understanding of the need or requirement. 
-Examples:  
-Example heading: “4.0 Alert Buzzer Requirements.”  
-Unacceptable: 4.1 The &lt;SOI&gt; shall sound it for greater than 20 minutes.   
-[This is unacceptable because the requirement uses the pronoun “it” (R24), which requires the 
-heading to understand what “it” means.  In addition, the word “sound” could be ambiguous as it 
-can be a noun, a verb, adverb, or adjective.  We do not know whether Alert_Buzzer is a 
-subsystem that controls the noise or the thing that makes the noise.] 
-Improved: When &lt;triggering event&gt;, the &lt;SOI&gt; shall sound an alert having the characteristics 
-defined in &lt;Alert Standard xyz&gt; for greater than 20 minutes. 
-[In this improved rewrite, the existence of the header is not needed to interpret the requirement.  
-Even though the above heading referenced an “Alert Buzzer”—an implementation, the improved 
-requirement avoids implementation to a specific device, and rather indicates that when the 
-triggering event happens, an alert is required to be sounded having the characteristics defined in 
-the alert standard. 
-Exceptions and relationships: 
-The use of headings is useful and acceptable when producing an output of an RMT, grouping like 
-types or categories of needs or requirements.  However, care must be taken that the headings 
-are used solely for management of the subsets of statements—the heading must not be 
-necessary to understand any of the grouped statements. See R41 and R42. 
-4.6 Realism 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid using unachievable absolutes. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall have 100% availability.   
-[This is unacceptable because 100% is an absolute that is impossible to achieve and verify.  
-Also, available over what time period?] 
-Improved: The &lt;SOI&gt; shall have an Availability of greater than or equal to 98% during 
-Operating_Hours. 
-[Note use of the glossary to define Operating_Hours. Alternatively, this requirement could be 
-stated as a need.  Then those transforming the need into requirements would develop a 
-_x000C_Guide to Writing Requirements 
-96 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-feasible concept for doing so and then derive specific Design Input Requirements that would 
-result in the need being met.] 
-Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 
-30 minutes.   
-[This is unacceptable because the requirement is impossibly precise to maintain in terms of the 
-flow rate (and impossibly precise to measure in verification) as well as being impossibly precise 
-to deliver for 30 minutes exactly. Also, it is not clear under what conditions this applies—when in 
-operations, when powered on, when commanded?] 
-Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters 
-per second for greater than 30 minutes.   
-[Now the range of acceptable flow performance and time frame is clear and feasible.  Given that 
-the condition “when in operations” this requirement applies whenever the Pumping_Station is 
-active—no matter how long. Also, what is the intent for how long—31 minutes satisfies the 
-requirement, but what if the real intent is for however long the Pumping Station is in operations 
-which could be hours or days—again depending on the operating conditions and need. Further, 
-is the 30 minutes of continuous flow or a total of 30 minutes within a set time period?] 
-4.7 Conditions 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-State conditions’ applicability explicitly instead of leaving applicability to be inferred from the 
-context. 
-Examples:  
-Unacceptable:  
-The Free_Access_Mode shall be set to ON within &lt;xxx ms&gt;. 
-The Fire_Door_Unlock command having the characteristics defined in &lt;ICD xyz&gt; shall be 
-sent to each Fire_Door within &lt;xxx ms&gt;. 
-[This is unacceptable because the condition or trigger for these actions is not stated. Also, note 
-the actions are written in passive voice which violates R2.  Each action needs to be 
-communicated in a separate active voice requirement statement with the condition or trigger for 
-which the action is to be initiated.  For multiple conditions for a single action see R28.] 
-Improved: (Split into two requirements) 
-In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode 
-to ON within &lt;xxx ms&gt;. 
-In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock 
-unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within 
-&lt;xxx ms&gt;. 
-[Note that there is a Fire Detection subsystem responsible for detecting fires and setting the 
-Fire_Detection parameter to “TRUE” which triggers the two actions.   All other subsystems that 
-are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” will 
-have their own requirements to monitor this parameter and take the required action(s) as stated 
-in their set of requirements.  All Fire Doors will have their own requirements to monitor for the 
-Fire_Door_Unlock command and to unlock when the command is received.] 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Express the propositional nature of a condition explicitly for a single action instead of giving lists of 
-actions for a specific condition. 
-Examples:  
-_x000C_Guide to Writing Requirements 
-98 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Unacceptable:  
-The Audit _Clerk shall be able to change the status of the action item when: 
- - the Audit _Clerk originated the item; 
- - the Audit _Clerk is the actionee; and 
- - the Audit _Clerk is the reviewer. 
-[This is unacceptable because it is not clear whether all the conditions must hold (a 
-conjunction) or any one of them (a disjunction).  Also, the requirement contains the phrase “be 
-able to” which violates R11.] 
-Better: If the requirement is interpreted as a disjunction:  
-The Audit_System shall change the Action_Item status requested by the Audit_Clerk when one 
-or more of the following conditions are true: 
- - the Audit_Clerk originated the Action_Item; 
- - the Audit_Clerk is the Actionee; or 
- - the Audit_Clerk is the Reviewer. 
-[Although the requirement is now improved, there is still the issue of verification. If the status 
-does not change with one of the listed conditions, then the entire requirement fails verification, 
-even if the other two conditions are met as specified.] 
-Better: In this case, it would be best to state three distinct requirements as this makes each 
-atomic and retains the same overall intent.  From an allocation, traceability, and verifiability 
-perspective this form is preferable. 
-The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
-Audit_Clerk originated the Action_Item. 
-The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
-Audit_Clerk is the Actionee. 
-The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
-Audit_Clerk is the Reviewer. 
-Better if interpreted as a conjunction:  
-The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
-following conditions are true: 
- - the Audit_Clerk originated the Action_Item AND 
- - the Audit_Clerk is the Actionee AND 
- - the Audit_Clerk is the Reviewer. 
-[In this form, the three conditions are expressed as a logical condition such that all three must 
-all be true for the logical condition to be true.] 
-4.8 Uniqueness 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Classify needs and requirements according to the aspects of the problem or system it addresses. 
-Examples:  
-Example classifications: Functional, Performance, Operational, Reliability, Availability, 
-Maintainability, Safety, Security, Design and Construction Standards, Physical Characteristics.  
-See the NRM for more guidance on organizing needs and requirements. 
-See Also R41 – Related Requirements 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Express each need and requirement once and only once. 
-Examples:  
-Exact duplicates can be found by matching of text strings.  The main problem is to identify 
-similarities with different expressions, but which are equivalent.   
-For example, the following statements are overlapping in that the first is a subset of the second: 
-The &lt;SOI &gt; shall generate a report of financial transactions containing the information defined in 
-&lt;some standard or contract deliverable listing&gt;. 
-The &lt;SOI&gt; shall generate a financial report. 
-4.9 Abstraction 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid stating implementation in a need statement or requirement statement unless there is 
-rationale for constraining the design. 
-Examples:  
-General: For a medical diagnostic system 
-• Stakeholders need statement: “The &lt;stakeholders&gt; need the &lt;diagnostic system&gt; to measure 
-[something] with an accuracy as good as or better than similar devices in the market.”  
-[This is an appropriate level of abstraction for a stakeholder need statement, clearly stating 
-the expectation the stakeholders have concerning accuracy, however this would not be a 
-good design input requirement.] 
-• Requirement transformed from the stakeholder need statement: “The &lt;diagnostic system&gt; 
-shall measure [something] with an accuracy of [xxx].”  
-[The developers have explored various concepts for meeting the need for accuracy, have 
-examined candidate technologies, have accessed their maturity (technology readiness level 
-(TRL), and have decided that the value [xxx] is feasible with acceptable risk for this lifecycle 
-stage.  As stated, this is an appropriate level of detail for a design input requirement.] 
-Note that when dealing with measures, both accuracy and precision must be addressed, either 
-as separate requirements or including both in a measurement requirement defining 
-characteristics of the measured parameter. 
-These system-level design input accuracy and precision requirements are then allocated to the 
-parts of the system architecture that have a role in meeting the overall system accuracy and 
-precision requirements.  For a medical diagnostic system this could include allocations to the 
-hardware (instrument), assay (biological sample), and software.  These allocations could then 
-be further sub-allocated within the hardware, assay, and software lower-level entities.   
-As long as the requirements are written on the accuracy and precision allocations and not how 
-that accuracy or precision will be obtained by one of the architectural entities, the requirements 
-are Design Input Requirements.  As soon as specific hardware components are named (laser, 
-LEDs emitting light at a specific wavelength, optical system components, specific 
-magnifications, algorithms, formulations, etc.,) then the requirements are reflecting design 
-outputs and need to be communicated within design output artifacts (specifications).  
-Unacceptable: Traffic lights shall be used to control traffic at the intersection.   
-[This is unacceptable because “Traffic lights” are a solution (design output).  Why are traffic 
-lights needed? This requirement is also written in passive voice - see R2] 
-Improved: (several requirements): 
-When a Pedestrian signals an intent to cross the street at the Intersection, the 
-Traffic_Control_System shall provide [the Pedestrian a “Walk” signal AND provide the traffic a 
-“Stop” signal]. 
-The Traffic_Control_System shall limit the Wait_Time of Vehicles traversing the Intersection to 
-less than Daylight_Wait_Time during Normal_Daytime traffic conditions.   
-[Note that glossary definitions should be used for Traffic_Control_System, 
-Daylight_Wait_Time_Value, Normal_Daytime, Vehicles, and Intersection.] 
-Unacceptable: When a pedestrian signals his presence by pressing a button on the traffic-light 
-pillar, the traffic light shall turn red for the traffic to stop.   
-[This is unacceptable because this requirement contains solution-biased detail - design output.  
-In addition, the requirement is unacceptable because it has additional information concerning 
-_x000C_Guide to Writing Requirements 
-102 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-the action traffic is to take and does not specify the duration of the red light.  The use of a 
-pronoun is also not recommended]. 
-Improved: When the presence of a Pedestrian that needs to cross the street at the Intersection 
-during Day_Light_Hours is detected, the Traffic_Control_System shall issue a 
-Traffic_Stop_Signal for Average_Pedestrian_Crossing_Time.  
-[This design input requirement allows freedom in determining the best solution (design output), 
-which may be a means of automatic detection rather than button pushing along with the type 
-and characteristics of the signal issued.  Note that pedestrians may be in proximity of the 
-intersection that do not wish to cross the street.]  
-[An interesting consideration from a consistency or conflict perspective, what if the 
-Average_Pedestrian_Crossing_Time” is greater than the “Daylight_Wait_Time_Value” defined 
-for the traffic in the previous example.  Each time is from a different entity perspective.] 
-[Note that glossary definitions should be used for “Pedestrian”, “Traffic_Control_System”, 
-“Traffic_Stop_Signal”, “Day_Light_Hours”, “Average_Pedestrian_Crossing_Time”, and 
-“Intersection”.] 
-Exceptions and relationships: 
-Sometimes solutions have to be described in requirements, even if it is very detailed for a given 
-level, for example if the airworthiness authorities require the use of a specific template for a 
-certain report; or if a naval customer requires that the new naval vessel be equipped with a 
-specific weapon system from a specific supplier; or if all vehicles in a fleet are required to use the 
-same fuel or the next model make use of a particular engine. In these cases, it is not a premature 
-solution, but a real stakeholder or customer need concerning a constraint.  As such this is 
-acceptable as a design input. 
-However, as a rule, if a detailed, specific design solution is expressed as a design input without 
-proper justification, it may be a premature solution and should be communicated as a design 
-output and an appropriate set of design input needs and associated requirements developed that 
-communicate “For what purpose?” which the design output requirements can be traced to.  
-Examples of issues concerning design outputs expressed as design inputs include: 
-1. The project is developing an upgrade to an existing system (brownfield SE).  Rather than 
-documenting design input “what” requirements, the project team focuses on known solutions 
-and implementations and documenting design output level requirements as design inputs.  
-This is problematic in that the real “for what purpose?” question is not being addressed and 
-the real Design Input Requirements are not communicated. 
-2. A similar case exists when procuring an off-the-shelf (OTS) solution and communicating the 
-requirements for that solution as Design Input Requirements rather than in a design output 
-specification.  Again, this is problematic in that the real “for what purpose?” question is not 
-being addressed and the real Design Input Requirements are not communicated. 
-3. A common issue arises when an existing system or OTS exists, yet the project develops 
-and documents as design inputs a detailed design output level set of requirements (design 
-output specification) for the system rather than a set of design input set of “what” 
-requirements that would guide the selection of an appropriate OTS.  This can result in a 
-redundant set of requirements that are not necessary, will have to be verified - adding 
-additional cost to the project, yet not addressing the “for what purpose?” design input 
-requirement set that should drive the selection of the specific OTS.  Refer to the NRM for a 
-detailed discussion the use of OTS entities. 
-_x000C_Guide to Writing Requirements 
-103 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-4. As part of the lifecycle concept analysis and maturation activities the project team developed 
-a prototype to access feasibility.  The resulting needs and resulting requirements are based 
-on the prototype and an associated trade study that resulted a specific solution that meets 
-the needs of the stakeholders.  Rather than communicating the Design Input Requirements, 
-the design output requirements for the prototype are included in the design input set of 
-requirements while not addressing the “for what purpose?” design input requirement set that 
-would drive the design for the prototype. 
-4.10 Quantifiers 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use “each” instead of “all”, “any”, or “both” when universal quantification is intended. 
-Examples:  
-Unacceptable: The Operation_Logger shall record any (or all) warning messages.   
-[This is unacceptable because of the use of the word “any”, which is then made worse by the 
-addition of “(or all)”.] 
-Improved: The Operation_Logger shall record each Warning_Message.   
-[Note that Warning_Message must be defined in the glossary so that it is clear that the SOI only 
-will record each defined Warning Message. Also, any conditions or performance must also be 
-included in the requirements statement for it to be complete.] 
-Unacceptable: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Names of 
-both of the Line_Items.   
-[This is unacceptable because of the use of the word “both”.] 
-Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Name of each 
-Line_Item.  
-Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; each 
-Line_Item_Name. 
-4.11 Tolerance 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Define each quantity with a range of values appropriate to the entity to which the quantity applies 
-and against which the entity will be verified or validated. 
-_x000C_Guide to Writing Requirements 
-104 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Examples:  
-Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 
-30 minutes.   
-[This is unacceptable because we do not know whether a solution that addresses more or less 
-than the specified quantities is acceptable Also, it is not clear under what conditions this applies 
-– when in operations, when powered on, when commanded?] 
-Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters 
-for a minimum of 30 minutes.   
-[Now the range of acceptable flow performance is clear and that the 30 minutes is a minimum 
-acceptable performance.  Given that the condition “when in operations”, this requirement applies 
-whenever the Pumping_Station is active—no matter how long. Also, a question to be asked is 
-what is the intent for how long—31 minutes satisfies the requirement, but what if the real intent is 
-for however long the Pumping Station is in operations which could be hours or days – again 
-depending on the operating conditions and need. What if there is not enough water at the inlet to 
-the pumping station to establish the required flow rate?] 
-Unacceptable: The Flight_Information_System shall display the current altitude to approximately 
-1 meter resolution.   
-[This is unacceptable because it is imprecise.  What is “approximately” in the context of a 
-distance of 1 meter?  Who has the option of deciding what is “approximately”?  How will 
-“approximately” be verified?  What is the acceptable tolerance?]  
-[Note that care must be taken to confirm that the units are appropriate in the context of the 
-organizational and project templates.  See also R6.] 
-Improved: The Flight_Information_System shall display Current_Altitude with an accuracy of ±1 
-meter.   
-[Note that “Current_Altitude” must be defined in the glossary since there are a number of 
-possible interpretations of the term.] 
-Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to allowable 
-levels.  Rationale: Arsenic contamination in drinking water can cause health problems.   
-[While “allowable” is acceptable in a need statement, it is unacceptable in a requirement 
-statement because allowable is ambiguous - allowable by whom?  What specific concentration 
-is allowable?  In what market?] 
-Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to 1 part per 
-trillion.  Rationale Attribute (A1): Arsenic contamination in drinking water can cause health 
-problems.   
-[This is unacceptable because the EPA contamination limit in drinking water is 10 parts per 
-billion.  Requiring a tighter limit may be beyond the ability of current technology to measure or 
-if measuring concentrations of 1 part per trillion are possible, the cost to do so may be 
-unacceptably high.  Also, no range is specified.  Using ‘less than’ is probably the real intent.] 
-Improved: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to less than10 parts 
-per billion.  Rationale Attribute (A1): EPA set the arsenic standard for drinking water at 10 ppb (or 
-0.010 parts per million).  The EPA has determined that concentrations of this level or less will 
-protect consumers from the effects of long-term, chronic exposure to arsenic. 
-Exceptions and relationships: 
-_x000C_Guide to Writing Requirements 
-106 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-The use of tolerances in need statements may not be as mandatory as their use in requirement 
-statements—see Appendix D. 
-4.12 Quantification 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Provide specific measurable performance targets appropriate to the entity to which the need or 
-requirement is stated and against which the entity will be verified to meet. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall use minimum power.   
-[This is unacceptable because both words “use” and “minimum” are ambiguous and 
-unverifiable.] 
-Improved: The &lt;SOI&gt; shall consume less than or equal to 50W of mains power.   
-[This both considers the underlying goal—to minimize power consumption—and provides a 
-measurable target.] 
-Unacceptable: The engine shall achieve an emissions level that is at least 5% less than the 
-competition’s emission levels 2 years from now.   
-[This is an actual requirement from marketing to an engineering department.  The statement 
-sets a completely unmeasurable end state.] 
-Improved: The Engine shall achieve an emissions level that is less than or equal to xxx.   
-[where xxx represents the required threshold value, including the appropriate units.] 
-Unacceptable: The &lt;SOI&gt; shall conform to best practices for spurious emissions. 
-[This statement is vague and unverifiable from number of specifics] 
-Improved: The &lt;SOI&gt; shall limit Spurious_Emissions in accordance with &lt;Clause xab of Standard 
-XYZ&gt;. 
-Exceptions and relationships: 
-Some quantification terms such as “minimum”, “maximum”, “optimal” are almost always 
-ambiguous.  Other terms may be ambiguous at lower levels but sufficient at the higher levels and 
-as need statements.  For example, it may be appropriate that the business state that “The Aircraft 
-shall provide class-leading comfort.”—while such a requirement is not quantifiable and therefore 
-not measurable, it may be sufficient for the business to communicate its intentions as a need 
-_x000C_Guide to Writing Requirements 
-107 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-statement to developers who can then turn comfort into such measurable quantities such as seat 
-dimensions and leg length.  
-This exception also applies to needs stated at the system or system element levels. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Define temporal dependencies explicitly instead of using indefinite temporal keywords such as 
-“eventually”, “until”, “before”, “after”, “as”, “once”, “earliest”, “latest”, “instantaneous”, 
-“simultaneous”, and “at last”. 
-Examples:  
-Unacceptable: Continual operation of the pump shall eventually result in the tank being empty.   
-[This is unacceptable because “eventually” is ambiguous.  Also, this statement is not written in 
-the proper form.  It is written on “operation” rather than on a requirement on the pump which 
-violates R3.] 
-Improved: The Pump shall remove greater than 99% of the Fluid from the Tank in less than 3 
-days of continuous operation. 
-4.13 Uniformity of Language 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use each term and unit of measure consistently throughout need and requirement sets as well as 
-associated models and other SE artefacts developed across the lifecycle. 
-Examples:  
-Unacceptable: It would not be acceptable for one requirement to refer to an entity using one term 
-and another to refer to the same entity using another term. 
-For example, a subsystem set of Design Input Requirements contains the following three 
-requirement statements: 
-    The Radio shall ....  
-    The Receiver shall .... 
-    The Terminal shall .... 
-Or: 
-    The Bleed_Valve shall ....  
-    The High-Pressure_Bleed_Valve shall .... 
-    The HPBV shall .... 
-If each term refers to the same subject, the statements need to be modified to use the same word 
-(or, if they are meant to be different, the words must be defined to be so). 
-Improved: Settle on only one term, define it in the glossary or data dictionary, and then use it 
-consistently in each need, requirement, and design output artifact. 
-Unacceptable: When the Input_Valve is connected to the Water_Source, the Control_Subsystem 
-shall open the Inlet_Valve.   
-[Two terms are used for the same thing “Input_Valve” and “Inlet_Valve”.] 
-Improved: When the Inlet_Valve is connected to the Water_Source, the Control_Subsystem shall 
-open the Inlet_Valve. 
-Unacceptable: It would not be acceptable for one requirement to use one unit of measure (for 
-example, US - feet) and another requirement to use another unit of measure (for example, Metric 
-- meter). 
-_x000C_Guide to Writing Requirements 
-109 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Improved: Settle on which units of measure will be used and use that unit of measure consistency 
-across all SE artifacts including needs, Design Input Requirements and design output 
-specifications.  
-Also, see R40 for guidance regarding the conversion from one measurement system to another 
-and the use of significant digits. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-If acronyms are used, they must be consistent throughout need and requirement sets as well as 
-associated models and other SE artefacts developed across the lifecycle. 
-Examples:  
-Unacceptable: It would not be acceptable for one requirement to use the acronym “CP” for 
-command post and another acronym “CMDP” to also refer to the “command post.” The use of two 
-different acronyms implies that the two system elements being referred to are different. 
-Improved: Settle on only one acronym, define it in the list of acronyms, and then use it 
-consistently throughout the requirement set. 
-Unacceptable: It would not be acceptable for one requirement to refer to the “Global Positioning 
-System” and the remaining requirements refer just to “GPS.” 
-Improved: Use the full term every time or, perhaps more usefully, define the acronym in the 
-project acronym list or glossary and use it every time. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Avoid the use of abbreviations in needs and requirement statements as well as associated 
-models and other SE lifecycle artefacts. 
-_x000C_Guide to Writing Requirements 
-110 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Examples:  
-Unacceptable: It would not be acceptable for one requirement to refer to the abbreviation “op” 
-meaning operation and another to refer to the “op” meaning the operator. 
-Improved: Avoid the abbreviation and use the full term every time. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use a project-wide style guide for individual need statements and requirement statements. 
-Examples:  
-For example, each organization should have a style guide or schema to address such issues as 
-the selection and definition of what need patterns and requirement patterns should be used for 
-writing need statements and requirement statements of a particular type, the selection and use of 
-attributes, standard abbreviations and acronyms, layout and use of figures and tables, layout of 
-documents or databases and, statement numbering.  
-_x000C_Guide to Writing Requirements 
-111 
-INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
-Terms used throughout the sets of needs and sets of requirements are defined in an ontology or 
-at least a project glossary. 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Use a consistent format and number of signification digits for the specification of decimal 
-numbers. 
-Examples:  
-Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp;  
-The &lt;SOI&gt; shall consume less than or equal to 0.99 W. 
-[These two statements are unacceptable when included in the same set because a different 
-format is used in the two statements.] 
-Improved:  
-The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp;  
-The &lt;SOI&gt; shall consume less than or equal to 0.99 W.  
-OR  
-The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp;  
-The &lt;SOI&gt; shall consume less than or equal to 0,99 W. 
-Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 0.99 h. &amp;  
-The &lt;SOI&gt; shall consume less than or equal to .99 W. 
-[These two statements are unacceptable when included in the same set because a different 
-format is used in the two statements.] 
-Improved:  
-The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp;  
-The &lt;SOI&gt; shall consume less than or equal to 0.99 W.  
-4.14 Modularity 
-4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  
-Group related needs and requirements together. 
-Examples:  
-Requirements may be related by: 
-- type (for example, critical functions, enabling functions, safety, or security requirements); 
-- scenario (for example, requirements arising from a single scenario). 
-- interactions with other systems (for example interface requirements). 
-- function (for example, multiple requirements defined for a function, each addressing a different 
-performance characteristics, mode, state, condition, or trigger.) 
-- capability (for example a needed capability may be released by a set of requirements that 
-together result in the needed capability to be provided. 
--compliance (for example requirements whose purpose it is to implement a requirement in a 
-standard or regulation. 
-See R29 and the NRM for more guidance on organizing needs and requirements. 
-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  
-Conform to a defined structure or template for organizing sets of needs and requirements. 
-Examples:  
 For sets of needs or requirements, an outline can be defined that organizes them in categories or 
 by type.   
 Examples of Type/Category of needs and requirements include:  
@@ -6832,13 +5419,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6869,20 +5456,8 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -6893,10 +5468,10 @@
         <v>1890</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>1890</v>
@@ -6905,31 +5480,19 @@
         <v>3631</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K2" t="s">
-        <v>224</v>
-      </c>
-      <c r="L2" t="s">
-        <v>266</v>
-      </c>
-      <c r="M2" t="s">
-        <v>267</v>
-      </c>
-      <c r="N2" t="s">
-        <v>266</v>
-      </c>
-      <c r="O2" t="s">
-        <v>268</v>
+        <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6940,10 +5503,10 @@
         <v>3636</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>3636</v>
@@ -6952,31 +5515,19 @@
         <v>7472</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K3" t="s">
-        <v>225</v>
-      </c>
-      <c r="L3" t="s">
-        <v>266</v>
-      </c>
-      <c r="M3" t="s">
-        <v>267</v>
-      </c>
-      <c r="N3" t="s">
-        <v>266</v>
-      </c>
-      <c r="O3" t="s">
-        <v>269</v>
+        <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6987,10 +5538,10 @@
         <v>7477</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>7477</v>
@@ -6999,31 +5550,19 @@
         <v>16353</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K4" t="s">
-        <v>226</v>
-      </c>
-      <c r="L4" t="s">
-        <v>266</v>
-      </c>
-      <c r="M4" t="s">
-        <v>267</v>
-      </c>
-      <c r="N4" t="s">
-        <v>266</v>
-      </c>
-      <c r="O4" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -7034,10 +5573,10 @@
         <v>16358</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>16358</v>
@@ -7046,31 +5585,19 @@
         <v>20821</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K5" t="s">
-        <v>227</v>
-      </c>
-      <c r="L5" t="s">
-        <v>266</v>
-      </c>
-      <c r="M5" t="s">
-        <v>267</v>
-      </c>
-      <c r="N5" t="s">
-        <v>266</v>
-      </c>
-      <c r="O5" t="s">
-        <v>271</v>
+        <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -7081,10 +5608,10 @@
         <v>20826</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <v>20826</v>
@@ -7093,31 +5620,19 @@
         <v>24520</v>
       </c>
       <c r="H6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K6" t="s">
-        <v>228</v>
-      </c>
-      <c r="L6" t="s">
-        <v>266</v>
-      </c>
-      <c r="M6" t="s">
-        <v>267</v>
-      </c>
-      <c r="N6" t="s">
-        <v>266</v>
-      </c>
-      <c r="O6" t="s">
-        <v>272</v>
+        <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -7128,10 +5643,10 @@
         <v>24525</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7">
         <v>24525</v>
@@ -7140,31 +5655,19 @@
         <v>29695</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K7" t="s">
-        <v>229</v>
-      </c>
-      <c r="L7" t="s">
-        <v>266</v>
-      </c>
-      <c r="M7" t="s">
-        <v>267</v>
-      </c>
-      <c r="N7" t="s">
-        <v>266</v>
-      </c>
-      <c r="O7" t="s">
-        <v>273</v>
+        <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -7175,10 +5678,10 @@
         <v>29700</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8">
         <v>29700</v>
@@ -7187,31 +5690,19 @@
         <v>33100</v>
       </c>
       <c r="H8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J8" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K8" t="s">
-        <v>230</v>
-      </c>
-      <c r="L8" t="s">
-        <v>266</v>
-      </c>
-      <c r="M8" t="s">
-        <v>267</v>
-      </c>
-      <c r="N8" t="s">
-        <v>266</v>
-      </c>
-      <c r="O8" t="s">
-        <v>274</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -7222,10 +5713,10 @@
         <v>33105</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F9">
         <v>33105</v>
@@ -7234,31 +5725,19 @@
         <v>34958</v>
       </c>
       <c r="H9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K9" t="s">
-        <v>231</v>
-      </c>
-      <c r="L9" t="s">
-        <v>266</v>
-      </c>
-      <c r="M9" t="s">
-        <v>267</v>
-      </c>
-      <c r="N9" t="s">
-        <v>266</v>
-      </c>
-      <c r="O9" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -7269,10 +5748,10 @@
         <v>34963</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <v>34963</v>
@@ -7281,31 +5760,19 @@
         <v>37730</v>
       </c>
       <c r="H10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J10" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K10" t="s">
-        <v>232</v>
-      </c>
-      <c r="L10" t="s">
-        <v>266</v>
-      </c>
-      <c r="M10" t="s">
-        <v>267</v>
-      </c>
-      <c r="N10" t="s">
-        <v>266</v>
-      </c>
-      <c r="O10" t="s">
-        <v>276</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -7316,10 +5783,10 @@
         <v>37735</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F11">
         <v>37735</v>
@@ -7328,31 +5795,19 @@
         <v>42493</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K11" t="s">
-        <v>233</v>
-      </c>
-      <c r="L11" t="s">
-        <v>266</v>
-      </c>
-      <c r="M11" t="s">
-        <v>267</v>
-      </c>
-      <c r="N11" t="s">
-        <v>266</v>
-      </c>
-      <c r="O11" t="s">
-        <v>277</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -7363,10 +5818,10 @@
         <v>42498</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F12">
         <v>42498</v>
@@ -7375,31 +5830,19 @@
         <v>44938</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K12" t="s">
-        <v>234</v>
-      </c>
-      <c r="L12" t="s">
-        <v>266</v>
-      </c>
-      <c r="M12" t="s">
-        <v>267</v>
-      </c>
-      <c r="N12" t="s">
-        <v>266</v>
-      </c>
-      <c r="O12" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -7410,10 +5853,10 @@
         <v>44943</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F13">
         <v>44943</v>
@@ -7422,31 +5865,19 @@
         <v>49509</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K13" t="s">
-        <v>235</v>
-      </c>
-      <c r="L13" t="s">
-        <v>266</v>
-      </c>
-      <c r="M13" t="s">
-        <v>267</v>
-      </c>
-      <c r="N13" t="s">
-        <v>266</v>
-      </c>
-      <c r="O13" t="s">
-        <v>279</v>
+        <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -7457,10 +5888,10 @@
         <v>49514</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14">
         <v>49514</v>
@@ -7469,31 +5900,19 @@
         <v>53099</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J14" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K14" t="s">
-        <v>236</v>
-      </c>
-      <c r="L14" t="s">
-        <v>266</v>
-      </c>
-      <c r="M14" t="s">
-        <v>267</v>
-      </c>
-      <c r="N14" t="s">
-        <v>266</v>
-      </c>
-      <c r="O14" t="s">
-        <v>280</v>
+        <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -7504,10 +5923,10 @@
         <v>53104</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F15">
         <v>53104</v>
@@ -7516,31 +5935,19 @@
         <v>55211</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="K15" t="s">
-        <v>237</v>
-      </c>
-      <c r="L15" t="s">
-        <v>266</v>
-      </c>
-      <c r="M15" t="s">
-        <v>267</v>
-      </c>
-      <c r="N15" t="s">
-        <v>266</v>
-      </c>
-      <c r="O15" t="s">
-        <v>281</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -7551,10 +5958,10 @@
         <v>55216</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F16">
         <v>55216</v>
@@ -7563,31 +5970,19 @@
         <v>58295</v>
       </c>
       <c r="H16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K16" t="s">
-        <v>238</v>
-      </c>
-      <c r="L16" t="s">
-        <v>266</v>
-      </c>
-      <c r="M16" t="s">
-        <v>267</v>
-      </c>
-      <c r="N16" t="s">
-        <v>266</v>
-      </c>
-      <c r="O16" t="s">
-        <v>282</v>
+        <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -7598,10 +5993,10 @@
         <v>58300</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F17">
         <v>58300</v>
@@ -7610,31 +6005,19 @@
         <v>61219</v>
       </c>
       <c r="H17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J17" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="K17" t="s">
-        <v>239</v>
-      </c>
-      <c r="L17" t="s">
-        <v>266</v>
-      </c>
-      <c r="M17" t="s">
-        <v>267</v>
-      </c>
-      <c r="N17" t="s">
-        <v>266</v>
-      </c>
-      <c r="O17" t="s">
-        <v>283</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -7645,10 +6028,10 @@
         <v>61224</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F18">
         <v>61224</v>
@@ -7657,31 +6040,19 @@
         <v>63959</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J18" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K18" t="s">
-        <v>240</v>
-      </c>
-      <c r="L18" t="s">
-        <v>266</v>
-      </c>
-      <c r="M18" t="s">
-        <v>267</v>
-      </c>
-      <c r="N18" t="s">
-        <v>266</v>
-      </c>
-      <c r="O18" t="s">
-        <v>284</v>
+        <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -7692,10 +6063,10 @@
         <v>63964</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F19">
         <v>63964</v>
@@ -7704,31 +6075,19 @@
         <v>72805</v>
       </c>
       <c r="H19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I19" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K19" t="s">
-        <v>241</v>
-      </c>
-      <c r="L19" t="s">
-        <v>266</v>
-      </c>
-      <c r="M19" t="s">
-        <v>267</v>
-      </c>
-      <c r="N19" t="s">
-        <v>266</v>
-      </c>
-      <c r="O19" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -7739,10 +6098,10 @@
         <v>72810</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F20">
         <v>72810</v>
@@ -7751,31 +6110,19 @@
         <v>75754</v>
       </c>
       <c r="H20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K20" t="s">
-        <v>242</v>
-      </c>
-      <c r="L20" t="s">
-        <v>266</v>
-      </c>
-      <c r="M20" t="s">
-        <v>267</v>
-      </c>
-      <c r="N20" t="s">
-        <v>266</v>
-      </c>
-      <c r="O20" t="s">
-        <v>286</v>
+        <v>238</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -7786,10 +6133,10 @@
         <v>75759</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F21">
         <v>75759</v>
@@ -7798,31 +6145,19 @@
         <v>78047</v>
       </c>
       <c r="H21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I21" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J21" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K21" t="s">
-        <v>243</v>
-      </c>
-      <c r="L21" t="s">
-        <v>266</v>
-      </c>
-      <c r="M21" t="s">
-        <v>267</v>
-      </c>
-      <c r="N21" t="s">
-        <v>266</v>
-      </c>
-      <c r="O21" t="s">
-        <v>287</v>
+        <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -7833,10 +6168,10 @@
         <v>78052</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F22">
         <v>78052</v>
@@ -7845,31 +6180,19 @@
         <v>80665</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J22" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K22" t="s">
-        <v>244</v>
-      </c>
-      <c r="L22" t="s">
-        <v>266</v>
-      </c>
-      <c r="M22" t="s">
-        <v>267</v>
-      </c>
-      <c r="N22" t="s">
-        <v>266</v>
-      </c>
-      <c r="O22" t="s">
-        <v>288</v>
+        <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -7880,10 +6203,10 @@
         <v>80670</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F23">
         <v>80670</v>
@@ -7892,31 +6215,19 @@
         <v>84721</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I23" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J23" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="K23" t="s">
-        <v>245</v>
-      </c>
-      <c r="L23" t="s">
-        <v>266</v>
-      </c>
-      <c r="M23" t="s">
-        <v>267</v>
-      </c>
-      <c r="N23" t="s">
-        <v>266</v>
-      </c>
-      <c r="O23" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -7927,10 +6238,10 @@
         <v>84726</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F24">
         <v>84726</v>
@@ -7939,31 +6250,19 @@
         <v>88927</v>
       </c>
       <c r="H24" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I24" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J24" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K24" t="s">
-        <v>246</v>
-      </c>
-      <c r="L24" t="s">
-        <v>266</v>
-      </c>
-      <c r="M24" t="s">
-        <v>267</v>
-      </c>
-      <c r="N24" t="s">
-        <v>266</v>
-      </c>
-      <c r="O24" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -7974,10 +6273,10 @@
         <v>88932</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F25">
         <v>88932</v>
@@ -7986,31 +6285,19 @@
         <v>91525</v>
       </c>
       <c r="H25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J25" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K25" t="s">
-        <v>247</v>
-      </c>
-      <c r="L25" t="s">
-        <v>266</v>
-      </c>
-      <c r="M25" t="s">
-        <v>267</v>
-      </c>
-      <c r="N25" t="s">
-        <v>266</v>
-      </c>
-      <c r="O25" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -8021,10 +6308,10 @@
         <v>91530</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F26">
         <v>91530</v>
@@ -8033,31 +6320,19 @@
         <v>93936</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I26" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J26" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K26" t="s">
-        <v>248</v>
-      </c>
-      <c r="L26" t="s">
-        <v>266</v>
-      </c>
-      <c r="M26" t="s">
-        <v>267</v>
-      </c>
-      <c r="N26" t="s">
-        <v>266</v>
-      </c>
-      <c r="O26" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -8068,10 +6343,10 @@
         <v>93941</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F27">
         <v>93941</v>
@@ -8080,31 +6355,19 @@
         <v>96507</v>
       </c>
       <c r="H27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I27" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J27" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="K27" t="s">
-        <v>249</v>
-      </c>
-      <c r="L27" t="s">
-        <v>266</v>
-      </c>
-      <c r="M27" t="s">
-        <v>267</v>
-      </c>
-      <c r="N27" t="s">
-        <v>266</v>
-      </c>
-      <c r="O27" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -8115,10 +6378,10 @@
         <v>96512</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F28">
         <v>96512</v>
@@ -8127,31 +6390,19 @@
         <v>99941</v>
       </c>
       <c r="H28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I28" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J28" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K28" t="s">
-        <v>250</v>
-      </c>
-      <c r="L28" t="s">
-        <v>266</v>
-      </c>
-      <c r="M28" t="s">
-        <v>267</v>
-      </c>
-      <c r="N28" t="s">
-        <v>266</v>
-      </c>
-      <c r="O28" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -8162,10 +6413,10 @@
         <v>99946</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F29">
         <v>99946</v>
@@ -8174,31 +6425,19 @@
         <v>103270</v>
       </c>
       <c r="H29" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I29" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K29" t="s">
-        <v>251</v>
-      </c>
-      <c r="L29" t="s">
-        <v>266</v>
-      </c>
-      <c r="M29" t="s">
-        <v>267</v>
-      </c>
-      <c r="N29" t="s">
-        <v>266</v>
-      </c>
-      <c r="O29" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -8209,10 +6448,10 @@
         <v>103275</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F30">
         <v>103275</v>
@@ -8221,31 +6460,19 @@
         <v>106159</v>
       </c>
       <c r="H30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I30" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J30" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K30" t="s">
-        <v>252</v>
-      </c>
-      <c r="L30" t="s">
-        <v>266</v>
-      </c>
-      <c r="M30" t="s">
-        <v>267</v>
-      </c>
-      <c r="N30" t="s">
-        <v>266</v>
-      </c>
-      <c r="O30" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -8256,10 +6483,10 @@
         <v>106164</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F31">
         <v>106164</v>
@@ -8268,31 +6495,19 @@
         <v>107763</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I31" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J31" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K31" t="s">
-        <v>253</v>
-      </c>
-      <c r="L31" t="s">
-        <v>266</v>
-      </c>
-      <c r="M31" t="s">
-        <v>267</v>
-      </c>
-      <c r="N31" t="s">
-        <v>266</v>
-      </c>
-      <c r="O31" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -8303,10 +6518,10 @@
         <v>107768</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F32">
         <v>107768</v>
@@ -8315,31 +6530,19 @@
         <v>117718</v>
       </c>
       <c r="H32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J32" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K32" t="s">
-        <v>254</v>
-      </c>
-      <c r="L32" t="s">
-        <v>266</v>
-      </c>
-      <c r="M32" t="s">
-        <v>267</v>
-      </c>
-      <c r="N32" t="s">
-        <v>266</v>
-      </c>
-      <c r="O32" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -8350,10 +6553,10 @@
         <v>117724</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F33">
         <v>117724</v>
@@ -8362,31 +6565,19 @@
         <v>119181</v>
       </c>
       <c r="H33" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I33" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J33" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="K33" t="s">
-        <v>255</v>
-      </c>
-      <c r="L33" t="s">
-        <v>266</v>
-      </c>
-      <c r="M33" t="s">
-        <v>267</v>
-      </c>
-      <c r="N33" t="s">
-        <v>266</v>
-      </c>
-      <c r="O33" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -8397,10 +6588,10 @@
         <v>119187</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F34">
         <v>119187</v>
@@ -8409,31 +6600,19 @@
         <v>126276</v>
       </c>
       <c r="H34" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I34" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="K34" t="s">
-        <v>256</v>
-      </c>
-      <c r="L34" t="s">
-        <v>266</v>
-      </c>
-      <c r="M34" t="s">
-        <v>267</v>
-      </c>
-      <c r="N34" t="s">
-        <v>266</v>
-      </c>
-      <c r="O34" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -8444,10 +6623,10 @@
         <v>126282</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F35">
         <v>126282</v>
@@ -8456,31 +6635,19 @@
         <v>128737</v>
       </c>
       <c r="H35" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I35" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J35" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K35" t="s">
-        <v>257</v>
-      </c>
-      <c r="L35" t="s">
-        <v>266</v>
-      </c>
-      <c r="M35" t="s">
-        <v>267</v>
-      </c>
-      <c r="N35" t="s">
-        <v>266</v>
-      </c>
-      <c r="O35" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -8491,10 +6658,10 @@
         <v>128743</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F36">
         <v>128743</v>
@@ -8503,31 +6670,19 @@
         <v>129760</v>
       </c>
       <c r="H36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I36" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J36" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="K36" t="s">
-        <v>258</v>
-      </c>
-      <c r="L36" t="s">
-        <v>266</v>
-      </c>
-      <c r="M36" t="s">
-        <v>267</v>
-      </c>
-      <c r="N36" t="s">
-        <v>266</v>
-      </c>
-      <c r="O36" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -8538,10 +6693,10 @@
         <v>129766</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F37">
         <v>129766</v>
@@ -8550,31 +6705,19 @@
         <v>134094</v>
       </c>
       <c r="H37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I37" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J37" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="K37" t="s">
-        <v>259</v>
-      </c>
-      <c r="L37" t="s">
-        <v>266</v>
-      </c>
-      <c r="M37" t="s">
-        <v>267</v>
-      </c>
-      <c r="N37" t="s">
-        <v>266</v>
-      </c>
-      <c r="O37" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:11">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -8585,10 +6728,10 @@
         <v>134100</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F38">
         <v>134100</v>
@@ -8597,31 +6740,19 @@
         <v>136241</v>
       </c>
       <c r="H38" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I38" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="K38" t="s">
-        <v>260</v>
-      </c>
-      <c r="L38" t="s">
-        <v>266</v>
-      </c>
-      <c r="M38" t="s">
-        <v>267</v>
-      </c>
-      <c r="N38" t="s">
-        <v>266</v>
-      </c>
-      <c r="O38" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -8632,10 +6763,10 @@
         <v>136247</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F39">
         <v>136247</v>
@@ -8644,31 +6775,19 @@
         <v>137370</v>
       </c>
       <c r="H39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J39" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K39" t="s">
-        <v>261</v>
-      </c>
-      <c r="L39" t="s">
-        <v>266</v>
-      </c>
-      <c r="M39" t="s">
-        <v>267</v>
-      </c>
-      <c r="N39" t="s">
-        <v>266</v>
-      </c>
-      <c r="O39" t="s">
-        <v>305</v>
+        <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:11">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -8679,10 +6798,10 @@
         <v>137376</v>
       </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F40">
         <v>137376</v>
@@ -8691,31 +6810,19 @@
         <v>139709</v>
       </c>
       <c r="H40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J40" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="K40" t="s">
-        <v>262</v>
-      </c>
-      <c r="L40" t="s">
-        <v>266</v>
-      </c>
-      <c r="M40" t="s">
-        <v>267</v>
-      </c>
-      <c r="N40" t="s">
-        <v>266</v>
-      </c>
-      <c r="O40" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:11">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -8726,10 +6833,10 @@
         <v>139715</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F41">
         <v>139715</v>
@@ -8738,31 +6845,19 @@
         <v>144325</v>
       </c>
       <c r="H41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J41" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K41" t="s">
-        <v>263</v>
-      </c>
-      <c r="L41" t="s">
-        <v>266</v>
-      </c>
-      <c r="M41" t="s">
-        <v>267</v>
-      </c>
-      <c r="N41" t="s">
-        <v>266</v>
-      </c>
-      <c r="O41" t="s">
-        <v>307</v>
+        <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:11">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -8773,10 +6868,10 @@
         <v>144331</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F42">
         <v>144331</v>
@@ -8785,31 +6880,19 @@
         <v>146369</v>
       </c>
       <c r="H42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I42" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="J42" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K42" t="s">
-        <v>264</v>
-      </c>
-      <c r="L42" t="s">
-        <v>266</v>
-      </c>
-      <c r="M42" t="s">
-        <v>267</v>
-      </c>
-      <c r="N42" t="s">
-        <v>266</v>
-      </c>
-      <c r="O42" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:11">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -8820,10 +6903,10 @@
         <v>146375</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E43" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F43">
         <v>146375</v>
@@ -8832,28 +6915,16 @@
         <v>148914</v>
       </c>
       <c r="H43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I43" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J43" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="K43" t="s">
-        <v>265</v>
-      </c>
-      <c r="L43" t="s">
-        <v>266</v>
-      </c>
-      <c r="M43" t="s">
-        <v>267</v>
-      </c>
-      <c r="N43" t="s">
-        <v>266</v>
-      </c>
-      <c r="O43" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to run_eval_loop algo
</commit_message>
<xml_diff>
--- a/aiswre/data/incose_guide_sections_df.xlsx
+++ b/aiswre/data/incose_guide_sections_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="310">
   <si>
     <t>start</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>examples</t>
+  </si>
+  <si>
+    <t>system_base_message</t>
+  </si>
+  <si>
+    <t>user_base_message</t>
+  </si>
+  <si>
+    <t>system_message</t>
+  </si>
+  <si>
+    <t>user_message</t>
   </si>
   <si>
     <t>4.1.1</t>
@@ -5031,6 +5043,1407 @@
   </si>
   <si>
     <t xml:space="preserve"> 
+For sets of needs or requirements, an outline can be defined that organizes them in categories or 
+by type.   
+Examples of Type/Category of needs and requirements include:  
+• 
+Function: Functional/Performance. 
+• 
+Fit: Operational: interactions with external systems - input, output, external interfaces, 
+operational environmental, facility, ergonomic, compatibility with existing systems, logistics, 
+users, training, installation, transportation, storage. 
+• 
+Quality (-ilities): reliability, availability, maintainability, accessibility, transportability, quality 
+provisions, growth capacity. 
+• 
+Form: physical characteristics. 
+• 
+Compliance:  
+– 
+Standards and regulations—policy and regulatory. 
+– 
+Constraints—imposed on the project and the project must show compliance. 
+– 
+Business rules—a rule imposed by the enterprise or business unit. 
+– 
+Business requirements—a requirement imposed by the enterprise or business unit. 
+Refer to the NRM Sections 4 and 6 for a more detailed discussion on this approach to organizing 
+needs and requirements. 
+Outlines for organizing needs and requirements can come from international standards or an 
+organizational standard tailored to the organization’s domain and different types of products 
+within that domain.  (The organization for system level needs and requirements may be different 
+than the organization of a set of software needs and requirements.) 
+</t>
+  </si>
+  <si>
+    <t>Step 1 - The user will hand over a Requirement, Criteria, and Examples. Your task is to revise the Requirement as per the provided Criteria and Examples, starting with the phrase "Initial Revision:".
+Step 2 - Compare the initial revision performed in Step 1 against the criteria to determine if any additional revisions are necessary. Let's think step-by-step.
+Step 3 - Return the final requirement revision based on Steps 1 and 2, starting with the phrase "Final Revision:".</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria: {definition}
+Examples: {examples}</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Need statements and requirement statements must conform to one of the agreed patterns, thus 
+resulting in a well-structured complete statement. 
+Examples:  
+See Appendix C, for examples of need statements and requirement statement patterns. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use the active voice in the need statement or requirement statement with the responsible entity 
+clearly identified as the subject of the sentence. 
+Examples:  
+Unacceptable: The Identity of the Customer shall be confirmed.   
+[This is unacceptable because it does not identify the entity that is responsible/accountable for 
+confirming the identity.] 
+Improved by adding the subject: The Identity of the Customer shall be confirmed by the 
+Accounting_System.   
+[Although this statement makes the subject clear, it is still unacceptable because the statement 
+is in the passive voice in that the entity that is responsible/accountable for recording the audio 
+is at the end of the statement rather than the beginning.] 
+Improved: The Accounting_System shall confirm the Customer_Identity. 
+_x000C_Guide to Writing Requirements 
+66 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+[Note that “Accounting_System”, “confirm”, and “Customer_Identity” must be defined in the 
+glossary since there are a number of possible interpretations of these terms—see R4. Also 
+note that this statement is improved because it is in the active voice but, before it is 
+acceptable, it needs to be further improved through the addition of appropriate condition and 
+qualifying clauses]  
+Unacceptable: While in the Operations_Mode, the Audio having the characteristics defined in 
+&lt;ICD xxxx&gt; shall be recorded.   
+[This is unacceptable because the entity that is responsible/accountable for recording the 
+audio is not stated, which makes it difficult to identify which entity is responsible for the action, 
+or how verification is to occur.  In addition, the characteristics of the Audio are not referenced, 
+nor are the conditions under which the action specified.] 
+Improved by adding the subject: While in the Operations_Mode, the Audio having the 
+characteristics defined in &lt;ICD xxxx&gt; shall be recorded by the &lt;SOI&gt;.   
+[Although this statement makes the subject clear, it is still unacceptable because the statement 
+is in the passive voice in that the entity that is responsible/accountable for recording the audio 
+is at the end of the statement rather than the beginning.] 
+Improved: While in the Operations_Mode, the &lt;SOI&gt; shall record Audio having the characteristics 
+defined in &lt;ICD xxxx&gt;.   
+[This is improved because it is in the active voice, but appropriate performance parameters 
+should be added before the statement is acceptable. Also note that “Audio” must be defined in 
+the glossary or data dictionary and required performance added for the requirement to be 
+complete. The characteristics of the Audio received from a &lt;xxxx&gt; source is defined in the 
+ICD.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Ensure the subject and verb of the need or requirement statement are appropriate to the entity to 
+which the statement refers. 
+Examples:  
+Subject examples: 
+Business management requirements have the form “The &lt;business&gt; shall …”.  For example, 
+“ACME_Transport shall …”. 
+Business operations requirements on business elements have the form “The &lt;business element&gt; 
+shall …”. For example, requirements on personnel roles have the form: “The &lt;personnel role&gt; 
+shall …”—such as, “The Production_Manager shall …”; “The Marketing_Manager shall …”. 
+System level needs have the form “The &lt;stakeholders&gt; need the system to ……” 
+System requirements have the form "The &lt;SOI&gt; shall ..."—for example, “The Aircraft shall …” 
+Subsystem level needs have the form “The &lt;stakeholders&gt; need the &lt;subsystem&gt; to ……” 
+Subsystem requirements have the form “The &lt;subsystem&gt; shall …" - for example, once the 
+subsystems are defined: “The Engine shall …”; and “The Landing_Gear shall …”. 
+Verb examples: 
+System level stakeholder need: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to process data received 
+from &lt;other system&gt;.” 
+System level requirement: “The &lt;SOI&gt; shall [process] data received from &lt;another system&gt;. 
+having the characteristics defined in &lt;Interface Definition XYZ.&gt;” 
+Through analysis, the verb/function “process” could be decomposed into sub functions such as 
+“receive”, “store”, “calculate”, “report”, and “display”.   
+Then a decision needs to be made regarding the specific subsystem or system element in which 
+these sub functions are to be performed.   
+If more than one subsystem or system element has a role in performing any one of the sub 
+functions, that requirement should be communicated at the system level and allocated to the 
+applicable subsystems or system elements.   
+If a sub function is to be implemented by a single subsystem or system element, then the sub 
+function requirement should be communicated at the subsystem or system element set of 
+requirements and traced back to the higher-level requirement from which it was decomposed. 
+Unacceptable system requirement: “The User shall ...”  
+[As discussed in Section 1.8, this is unacceptable because the requirement should be on the 
+system, not the user or operator of the system.  This wording is often the result of writing 
+requirements directly from user stories or resulting need statements, without doing the 
+_x000C_Guide to Writing Requirements 
+69 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+transformation of the use case or need into a requirement.  Ask, what does the system have to 
+do so that the need can be achieved?] 
+Improved: “The &lt;SOI&gt; shall …”. 
+Unacceptable: The &lt;SOI&gt; shall display the Current_Time on the &lt;Display Device&gt; per &lt;Display 
+Standard xyz&gt;.   
+[Again, “Current_Time” and “Display_Device” must be defined in the glossary or data 
+dictionary. This statement is most likely unacceptable because the Display_Device is either a 
+system element which is presumably at a level lower than the SOI (and is therefore not 
+appropriate to this level), or the Display_Device is a system or system element outside the SOI 
+(and therefore should be handled as an interface since requirements cannot be placed on it by 
+this requirement set). The display standard would be developed by the organization that would 
+define standards to be used when displaying all information by all applications the organization 
+develops including fonts, font sizes, colors, spacing, brightness, human factors, etc.] 
+Improved: The &lt;SOI&gt; shall display the Current_Time per &lt;Display Standard xyz&gt;.   
+[This is improved because the action is appropriate to the level of the requirement set. Note 
+that, before being an acceptable statement, appropriate condition and qualifying clauses must 
+be added.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Define all terms used within the need statement and requirement statement within an associated 
+glossary and/or data dictionary. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall display the current time as defined in &lt;Display Standard xyz&gt;.   
+[This is unacceptable because it is ambiguous. What is “current”? In which time zone? To what 
+degree of accuracy? In which format?] 
+Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;Display Standard xyz&gt;.   
+[Note that “Current_Time” must then be defined in the glossary or data dictionary in terms of 
+accuracy, format, time zone, and units. Further, appropriate condition and qualifying clauses 
+must be included before the statement is acceptable.  In addition, the organization can define a 
+display standard that applies to all products developed by the organizations concerning how 
+information is to be displayed (fonts, colors, size, spacing, human factors, etc.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use the definite article “the” rather than the indefinite article “a”. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall provide a time display.   
+[This is unacceptable for a requirement because it is ambiguous—is the intent to provide a 
+device to display the time or to display the time? If a device to display the time, then this is not 
+appropriate to level.  If to display a time - will any time displayed do?  Is a one-off display of the 
+time satisfactory?  The writer's intention was most likely that they wanted the system to display 
+continuously the current time in a format that is readable, yet if the developer provided a 
+constant display of “10:00 am” (or even a one-off display of any time), they could argue (albeit 
+unreasonably) that they have met the requirement; yet they would have clearly failed to meet 
+the customer's need and intent. 
+Note that, as a need statement: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to display the time.”, the 
+statement is arguably acceptable.  However, as part of the transformation process, the 
+requirement writers must remove the ambiguity - resulting in the following requirement 
+statement (amongst others). 
+Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;display standard xyz&gt;.   
+[Note that “Current_Time” must be defined in the glossary or data dictionary since there are a 
+number of possible meanings and formats of the more-general term “current time.” For 
+completeness, condition and qualifying clauses must also be added before the requirement is 
+acceptable. In addition, the organization can define a standard that applies to all products 
+developed by the organizations concerning how information is to be displayed (fonts, colors, 
+size, spacing, human factors, etc.]  
+Exceptions and relationships: 
+The purpose of this rule is to avoid the ambiguity that arises because “a” or “an” is tantamount to 
+saying, “any one of”.  In some cases, however, the use of an indefinite article is not misleading.  
+For instance, “… with an accuracy of less than 1 second” allows the phrase to read more 
+naturally and there is no ambiguity because of the accuracy quoted. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+When stating quantities, all numbers should have appropriate and consistent units of measure 
+explicitly stated using a common measurement system in terms of the thing the number refers. 
+_x000C_Guide to Writing Requirements 
+72 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Examples:  
+Unacceptable: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 
+degrees.   
+[This is unacceptable because the units used are stated without indicating the specific 
+measurement system used.] 
+Improved: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 degrees 
+Celsius. 
+Unacceptable: The &lt;SOI&gt; shall establish communications as defined in &lt;ICD xyz&gt; with at least 4 
+in less than or equal to 10 seconds.   
+[This is unacceptable because the units used are incomplete.  “4” of what?] 
+Improved: The &lt;SOI&gt; shall &lt;establish communications&gt; as defined in &lt;ICD xyz&gt; with at least 4 
+satellites in less than or equal to 10 seconds  
+_x000C_Guide to Writing Requirements 
+73 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+[Note that the phrase “establish communications” is probably acceptable at the business level 
+when used in a need statement, but the phrase would need further elaboration at lower levels so 
+that the need is decomposed into verifiable requirements relating to frequency, type of 
+communications (voice? data?), quality, bandwidth, etc. which would typically be defined in an 
+ICD that defines the characteristics of the communication signal to be established.] 
+Unacceptable:  
+“The Fuel_System shall have a maximum fuel volume of 60 l”.   
+“When the Fuel_System detects the Fuel_Tank volume is less than 500 ml, the Fuel_System shall 
+notify the operator within 1 second.” 
+[This is unacceptable because the two requirements use different units of measure (“l” and “ml”). 
+Improved:  
+“The Fuel_System shall have a maximum Fuel_Tank volume of 60 l “.   
+“When the Fuel_System detects the Fuel_Tank volume is less than 0.5 l, the Fuel_System shall 
+notify the operator within 1 second.” 
+[Now both requirements are written using the same units of measure(liters).] 
+Additional Acceptable: "The Fuel_System shall have a maximum Fuel_Tank volume of 60 l.” “When 
+the Signal_System detects the Fuel_Tank volume is less than 50 ml, the Signal_System shall light 
+the Low-Fuel_Iindicator within 1 second." 
+[In this particular case, while the property (“Fuel_Tank volume”) remains the same, the 
+component/element is different ("Fuel_System" vs "Signal_System"). The measurement unit can 
+vary because we are dealing with different component–property pairs.] 
+[Note that “Fuel_System” and “Fuel_Tank” must be defined in the glossary or data dictionary.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the use of vague terms. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall usually be online.   
+[This is unacceptable because “usually” is ambiguous - is availability what is meant?] 
+Improved: The &lt;SOI&gt; shall have an Availability of greater than xx% over a period of greater than 
+yyyy hours.   
+[Note that “Availability” must be defined in the glossary or data dictionary since there are a 
+number of possible ways of calculating that measure.  Alternately, the availability could be 
+expressed as a need.  Then the organization responsible for transforming the need into a 
+requirement could develop feasible concepts for meeting the needed availability and derived 
+one or more well-formed requirements that result in the need being met.] 
+Unacceptable: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the 
+Tracking_Information for relevant aircraft within &lt;xxxx seconds&gt; of detection. 
+[This is unacceptable because it does not make explicit which aircraft are relevant.  Additionally, 
+the statement allows the developer to decide what is relevant; such decisions are in the 
+province of the customer, who should make the requirement explicit.] 
+Improved: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the 
+Tracking_Information of each Aircraft located less than or equal to 20 kilometers from the Airfield 
+when in the Operations_Mode within &lt;xxxx seconds&gt; of detection.   
+[Now it is clear for which aircraft the information needs to be displayed.  Note that “Aircraft”, 
+“Tracking_Information”, “Airfield”, and “Operations_Mode” must be defined in the glossary or 
+data dictionary.] 
+Exceptions and relationships: 
+R3 points out that the use of a verb such as “safe”, may be acceptable at the business 
+management or operations level as long as it is unambiguous at that level, decomposed at the 
+lower levels, and is verifiable at the level stated.  Similarly, some vague adjectives may be 
+allowable at the business management or operations level, providing they are not ambiguous at 
+that level. NLP/AI tools providing automatic assessment of this rule shall be flexible enough and 
+tailorable in order not to identify this issue as an error at a business level, while enforcing the 
+absence of vague terms in other lower-level documents. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the inclusion of escape clauses that state vague conditions or possibilities, such as “so far as is 
+possible”, “as little as possible”, “where possible”, “as much as possible”, “if it should prove 
+necessary”, “if necessary”, “to the extent necessary”, “as appropriate”, “as required”, “to the extent 
+practical”, and “if practicable”. 
+Examples:  
+Unacceptable: The GPS shall, where there is sufficient space, display the User_Location in 
+accordance with &lt;Display Standard xyz&gt;.   
+[This is unacceptable because whether there is sufficient space is vague, ambiguous, and 
+unverifiable.  The requirement is clearer without the escape clause.]  
+Improved: The GPS shall display the User_Location in accordance with &lt;Display Standard XYZ&gt;. 
+[Note that appropriate performance measures must also be specified such as within what time, 
+format, and accuracy.  Also note that “GPS” and “User_Location” must be defined in the 
+glossary or data dictionary.]   
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid open-ended, non-specific clauses such as “including but not limited to”, “etc.” and “and so 
+on”. 
+Examples:  
+Unacceptable: The ATM shall display the Customer Account_Number, Account_Balance, and so 
+on per &lt;Display Standard xyz&gt;.   
+[This is unacceptable because it contains an opened list of what is to be displayed.] 
+_x000C_Guide to Writing Requirements 
+76 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Improved: [Split into as many requirements as necessary to be complete.  Note that the types of 
+customer information to be displayed needs to be defined in the glossary.]: 
+The ATM shall display the Customer Account_Number in accordance with &lt;Display Standard 
+xyz&gt;. 
+The ATM shall display the Customer Account_Balance in accordance with &lt;Display Standard 
+xyz&gt;. 
+The ATM shall display the Customer Account_Type in accordance with &lt;Display Standard 
+xyz&gt;. 
+The ATM shall display the Customer Account_Overdraft_Limit in accordance with &lt;Display 
+Standard xyz&gt;. 
+[Note: Some may feel that a bulleted list or table is acceptable.  While, from a readability 
+perspective, this may be true, from a requirement management perspective, each item in the 
+bulleted list is still a requirement.  Because of this requirement statements as in the example 
+above should be written as individual statements especially when allocation, traceability, 
+verification, and validation activities are specific to the single item.  See also R17, R18, R22, 
+and R28.] 
+[Note the above examples are incomplete in that expected performance and under what 
+conditions has not been included in the requirement statements.] 
+4.2 Concision 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the use of superfluous infinitives such as “to be designed to”, “to be able to”, “to be capable 
+of”, “to enable”, “to allow”. 
+Examples:  
+Unacceptable: The Weapon_System shall be able to store the location of each Ordnance.   
+[This is unacceptable because it contains the superfluous infinitive “be able to” which implies the 
+requirement is ubiquitous in that it can be applied at any time, but it therefore begs the question 
+as to the condition under which the feature can be invoked.  However, this is acceptable for the 
+stakeholder need: “The stakeholders need the Weapon_System to be able to store the location 
+of each Ordnance.”] 
+Improved: When &lt;condition&gt;he Weapon_System shall store the Location of each Ordnance.   
+[This is better because the requirement applies only in a particular condition. Note that the 
+terms “Weapon_System”, “Location”, and “Ordnance” must be defined in the glossary or data 
+dictionary. To be complete the appropriate performance characteristics would also need to be 
+defined and included within the requirement statement.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use a separate clause for each condition or qualification. 
+Examples:  
+Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the 
+characteristics defined in &lt;ICD xyz&gt; at an accuracy of less than or equal to 20 meters to each 
+Maritime_User during Harbor_Harbor_Approach_Maneuvering (HHAM).   
+[This is unacceptable because it inserts a phrase in such a way that the object of the sentence 
+is separated from the verb.] 
+Improved: The Navigation_Beacon shall provide Augmentation_Data having the characteristics 
+defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering 
+(HHAM), at an accuracy of less than or equal to 20 meters.   
+[This rewrite places the basic function in an unbroken clause followed by the sub-clause 
+describing performance.  Note that: “Navigation_Beacon”, “Maritime_User”, and 
+“Harbor_Harbor_Approach_Maneuvering (HHAM)” must be defined in the glossary or data 
+dictionary. There is also an issue in that when discussing accuracy, precision needs to also be 
+addressed.] 
+4.3 Non-ambiguity 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use correct grammar. 
+Examples:  
+Unacceptable: The Weapon_System shall storing the location of all ordnance.   
+[This is unacceptable because the grammatical error leads to uncertainty about the meaning.] 
+Improved: The Weapon_System shall store the location of all Ordnance.   
+[Note that “Ordnance” must be defined in the glossary to be explicit about the types of weapons 
+and ammunition. Also, where the location is to be stored and the format of the data, must be 
+addressed. The action “store” needs to be further evaluated to determine if that is an 
+appropriate action (verb) for the Weapon_System vs a user interacting with the 
+Weapon_System as discussed in R3.  Additionally, to be complete any specific performance 
+measures and conditions should be included within the requirement statement.] 
+Unacceptable: When in the Active_State, the Record_Subsystem shall display each of the 
+Names of the Line_Items, without obscuring the User_ID per &lt;Display Standard xyz&gt;. 
+[This is unacceptable because the grammatical error involving the inappropriate placement of 
+“each of”—it is most likely that a Line_Item has only one name.] 
+Improved: When in the Active_State, the Record_Subsystem shall display on &lt;Display Device&gt; 
+the Name of each Line_Item, without obscuring the User_ID per &lt;Display Standard XYZ.&gt;.  
+[This is acceptable the ambiguity has been addressed.  The requirement is now more complete 
+in that it references where the information is to be display and the standard to be used 
+concerning the display of the information. If there are any performance measures that apply, 
+they would also need to be addressed.] 
+Unacceptable: The &lt;corporate website&gt; shall only use Approved_Fonts. 
+[This is unacceptable because it mandates that the website shall only use the designated 
+fonts—that is, it is not expected to perform any other function except to use those fonts. This is 
+clearly not what is meant but becomes ambiguous by the inappropriate grammar and the 
+incorrect placement of the word “only”. What is most likely meant is that the only fonts to be 
+used are the approved fonts defined in the organization’s display standard.] 
+Improved: The &lt;corporate website&gt; shall display information using Approved_Fonts defined in 
+&lt;Display Standard xyz&gt;. 
+_x000C_Guide to Writing Requirements 
+80 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+[This is better because the ambiguity has been addressed.  To be acceptable, any conditions 
+and qualifying clauses would also need to be added.  If the organization has a standard for 
+displaying information that addresses acceptable fonts, font sizes, colors, spacing, human 
+factors, etc., the requirement should refer to that standard.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use correct spelling. 
+Examples:  
+Unacceptable: The Weapon_System shall store the location of each ordinance.   
+[This is unacceptable because the word “ordinance” means regulation or law.  It is unlikely that 
+the Weapon_System is interested in the location of ordinance (regulations).  In the context of a 
+_x000C_Guide to Writing Requirements 
+81 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+weapon system, what the authors meant to use is "ordnance" as in weapons and ammunition, 
+not “ordinance”.] 
+Improved: The Weapon_System shall store the Location of each Ordnance.   
+[Note that “Location” and “Ordnance” must be defined in the glossary or data dictionary to be 
+explicit about the types of weapons and ammunition.  The action “store” needs to be further 
+evaluated to determine if that is an appropriate action (verb) for the Weapon_System vs a user 
+interacting with the Weapon_System as discussed in R3.  Additionally, to be complete any 
+specific performance measures and conditions should be included within the requirement 
+statement.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use correct punctuation. 
+Examples:  
+Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the 
+characteristics defined in &lt;ICD xyz&gt; to each Maritime_User, engaged in 
+Harbor_Harbor_Approach_Maneuvering (HHA) at an accuracy of less than 20 meters.   
+[This is unacceptable because the incorrectly placed comma in this sentence confuses the 
+meaning, leading the reader to believe that the accuracy is related to the maneuver rather than 
+to the augmentation data.]  
+Improved: The Navigation_Beacon shall provide Navigation_Data having the characteristics 
+defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering 
+(HHA), at an accuracy of less than 20 meters. 
+[The positioning of the comma now makes it clear that the accuracy and availability relate to the 
+data. Also note that, while performance measures are included, the appropriate conditions are 
+not addressed.  Further “Navigation_Beacon”, “Navigation_Data”, “Maritime_User”, and 
+“Harbor_Harbor_Approach_Maneuvering (HHA)” must be defined in the glossary or data 
+dictionary.]  
+_x000C_Guide to Writing Requirements 
+82 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use a defined convention to express logical expressions such as “[X AND Y]”, “[X OR Y]”,  
+[X XOR Y]”, “NOT [X OR Y]”. 
+Examples:  
+Unacceptable: The Engine_Management_System shall disengage the 
+Speed_Control_Subsystem within &lt;TBD seconds&gt; when the Cruise_Control is engaged, and the 
+Driver applies the Accelerator.   
+[This is unacceptable because of the ambiguity of “and” could be confused with combining two 
+separate thoughts.  Instead use the form of a logical expression [X AND Y].] 
+Improved: When [the Cruise_Control is Engaged] AND [the Accelerator is Applied], the 
+Engine_Management_System shall Disengage the Speed_Control_Subsystem within &lt;TBD 
+seconds&gt;.  
+[“Engine_Management_System”, “Speed_Control_Subsystem”, “Disengage”, “Engaged”, 
+“Accelerator”, “Applied”, and “Cruise_Control” must be defined in the glossary or data dictionary.] 
+_x000C_Guide to Writing Requirements 
+83 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Exceptions and relationships: 
+While R21: Avoid Parentheses states that parentheses or brackets are to be avoided within 
+general sentence structure, this rule suggests that brackets may be used as part of a convention to 
+avoid ambiguity when expressing a logical expression.   
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the use of the word “not”. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall not fail.   
+[This is unacceptable because verification of the requirement would require infinite time. The 
+requirement is also infeasible in that, as written, the implication is to never fail, under any 
+conditions.] 
+Improved:  
+The &lt;SOI&gt; shall have an Availability of greater than or equal to 95%.  or  
+The &lt;SOI&gt; shall have a Mean Time Between Failures (MTBF) of xx operating hours. 
+[For quality requirements, it would be more precise in the above were written as need 
+statements.  Then those transforming the quality need statements into requirement statements 
+would define feasible concepts that would result in the needed quality attributes and derive well-
+formed requirements on the &lt;SOI&gt; that would result in those needs to be met.] 
+Unacceptable: The &lt;SOI&gt; shall not contain mercury.   
+[This is unacceptable because verification of the requirement would require the ability to 
+measure the amount of mercury with infinite accuracy and precision.  In addition, the real 
+requirement may not be stated, for example, the real concern may be the use of toxic materials, 
+not just mercury.  If that is the case, it may be best to reference a standard from a governmental 
+agency concerning allowable exposures to a list of common toxic materials.] 
+Improved: The &lt;SOI&gt; shall limit metallic mercury exposure to those coming in contact with the 
+&lt;SOI&gt; to less than or equal 0.025 mg/m3 over a period of 8 hours. 
+Exceptions and relationships: 
+It may be reasonable to include “not” in a requirement when the logical “NOT” is implied—for 
+example when using not [X or Y].  In that case, however, in accordance with R15, it may be better 
+to capitalize the “NOT” to make the logical condition explicit: NOT [X or Y].   
+_x000C_Guide to Writing Requirements 
+84 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+There may be other cases such as “The &lt;SOI&gt; shall not be red in color.”, which is stating a 
+constraint and is verifiable, as long as the range of shades of red is stated (RBG rr,bb,gg range or 
+a “name” of red in some standard).   
+The key consideration is verification.  If the “not” can be unambiguously verified, then its use is 
+acceptable. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the use of the oblique (“/”) symbol. 
+Examples:  
+Unacceptable: The User_Management_System shall Open/Close the User_Account in less than 
+1 second.   
+[This is unacceptable because it is unclear as to what is meant by open/close: open, close, or 
+both?] 
+Improved: (Split into two requirements with an appropriate condition)  
+When &lt;condition&gt;, the User_Management_System shall Open the User_Account in less than 1 
+second. 
+When &lt;condition&gt;, the User_Management_System shall Close the User_Account in less than 1 
+second.  
+Unacceptable: When the Clutch is Disengaged and/or the Brake is Applied, the 
+Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;.   
+[This is unacceptable because of the use of “and/or.” If simultaneity is intended—that is the dual 
+conditions must be met at the same time—write the requirements as a logical AND. If “and” is 
+meant in the sense that the action is to be completed under each of the conditions, split the two 
+thoughts into separate requirements, one for each condition.  If “or” is meant, write the 
+requirement as a logical OR.] 
+Improved: (As one requirement if simultaneity is intended): 
+When [the Clutch is Disengaged] AND [the Brake is Applied], the Engine_Management_System 
+shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. 
+_x000C_Guide to Writing Requirements 
+85 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Improved: (As two requirements if two separate conditions are intended): 
+When the Clutch is Disengaged, the Engine_Management_System shall disengage the 
+Speed_Control_Subsystem within &lt;XYZ ms&gt;. 
+When the Brake is Applied, the Engine_Management_System shall disengage the 
+Speed_Control_Subsystem within &lt;XYZ ms&gt;. 
+Improved: (As one requirement if inclusive OR is intended)  
+When EITHER [the Clutch is Disengaged] OR [the Brake is Applied], the 
+Engine_Management_System shall disengage the Speed_Control_Subsystem. 
+4.4 Singularity 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Write a single sentence that contains a single thought conditioned and qualified by relevant sub-
+clauses. 
+Examples:  
+Unacceptable:  When in the Active_State, the Record_Subsystem shall display the Name of each 
+Line_Item and shall record the Location of each Line_Item, without obscuring the User_ID.   
+[This is unacceptable because the sentence contains two requirements and the qualification 
+only applies to the first requirement, not the second.] 
+Improved: (Split into two separate requirements)  
+When in the Active_State, the Record_Subsystem shall display per &lt;Display Standard XYZ&gt; 
+the Name of each Line_Item, without obscuring the User_ID.  
+When in the Active_ State, the Record_Subsystem shall record the Location of each Line_Item. 
+[Note use of the glossary or data dictionary to define terms.  Any applicable performance 
+measures must be addressed for the requirement to be complete.] 
+Unacceptable: The Control_Subsystem will close the Inlet_Valve until the temperature has 
+reduced to 85 °C, when it will then reopen it in less than 1 second.   
+[This is unacceptable because the sentence contains two event driven requirements.  
+Additionally, the sentence contains two occurrences of the pronoun “it” ambiguously referring to 
+different things (see R26), the term “has reduced” is ambiguous, and the action verb must be 
+”shall”, not “will”. Also, a time constraint is included but it is not clear whether it applies to both 
+actions or only the second action.] 
+Improved: (Split into two requirements each with its own time constraint): 
+If the Water_Temperature in the Boiler increases to greater than 85 °C, the Control_Subsystem 
+shall close the Inlet_Valve in less than 1 second.  
+When the Water_Temperature in the Boiler reduces to less than or equal to 85 °C, the 
+Control_Subsystem shall open the Inlet_Valve in less than 1 second. 
+[Note use of the glossary or data dictionary to define terms.]  
+Unacceptable:  
+In the event of a fire detection, within &lt;xxx ms&gt;: 
+• 
+Security entrances shall be set to Free_Access_Mode. 
+• 
+Fire escape doors shall be unlocked. 
+[This is unacceptable because the condition “in the event of a fire detection” is stated following a 
+list of actions to be taken; each of which the system must be verified against.  Also, note the 
+actions are written in passive voice which violates R2.  Each action needs to be communicated 
+in a separate active voice requirement statement.  For multiple conditions for a single action see 
+R28.] 
+Improved: (Split into two requirements) 
+In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode 
+to ON within &lt;xxx ms&gt;. 
+In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock 
+unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within 
+&lt;xxx ms&gt;. 
+[There is a Fire Detection subsystem responsible for detecting fires and setting the 
+Fire_Detection parameter to “TRUE” which triggers the two actions.   All other subsystems that 
+_x000C_Guide to Writing Requirements 
+87 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” 
+will take the required action as stated in their set of requirements.  All Fire Doors will be 
+monitoring for the Fire_Door_Unlock command and will unlock when the command is 
+received.] 
+Unacceptable: The &lt;corporate website&gt; shall use only approved fonts. The approved fonts are: 
+&lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;. 
+[This is unacceptable because it is non-singular. Rather than splitting into three requirements 
+(which is quite difficult to so whilst conforming to the “only” constraint, the term 
+“Approved_Fonts” can be included in the Glossary, which then states: “Approved_Fonts: 
+&lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;.”] 
+Improved: (using the glossary term “Approved_Fonts”) 
+The &lt;corporate website&gt; shall use only Approved_Fonts.  
+[Alternately, the organization can define a display standard which includes a definition of 
+approved fonts, and the requirement could reference that standard.] 
+Improved: (referring to a standard.) 
+The &lt;corporate website&gt; shall display information in accordance with &lt;Display Standard xyz&gt;. 
+[Note that this also allows better configuration management of the requirements database, 
+particularly if the approved fonts are referred to in a number of requirements—that is, should 
+the approved fonts change or characteristics of the fonts change, the list of approved fonts and 
+characteristics only needs to be updated in the Glossary, rather than in multiple requirements 
+(in which case there is a risk that one or more of the requirements is missed).] 
+[In reality, requirements involving the actions such as “display” are interface requirements 
+given that the information will be provided by something to some display device for display.] 
+[Having the information in the display standard then can be referred to in the set of 
+requirements for that display device. Note that referring to a standard also allows for later 
+specialization, for example different parts of the standard may apply to different display 
+devices.] 
+Exceptions and relationships: 
+Every requirement should have a main clause with a main verb (R1).  However, additional sub-
+clauses with auxiliary verbs or adverbs may be used to qualify the requirement with performance 
+attributes. 
+Such sub-clauses cannot be verified in isolation since they are incomprehensible without the 
+main clause.  Sub-clauses that need to be verified separately from others should be expressed as 
+separate requirements. 
+For example, “The Ambulance_Control_System shall communicate Incident_Details to the Driver” 
+is a complete, comprehensible statement with a single main verb.  An auxiliary clause may be 
+added to provide a qualifying constraint “The Ambulance_Control_System shall communicate 
+Incident_Details to the Driver, while simultaneously maintaining communication with the Caller.”  
+[Note: the verb “communicate” is more appropriate for a need statement.  The resulting Design 
+Input Requirements would address the specific means of communication.] 
+_x000C_Guide to Writing Requirements 
+88 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Similarly, if the requirement is to extinguish and dispose of a match as a single combined action, 
+the requirement must ensure that both are verified the same time and allocated the same. 
+Note that, if performance attributes need to be verified separately, they should be expressed as 
+sub-clauses in separate requirements.   
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid words that join or combine clauses, such as “and”, “or”, “then”, “unless”, “but”, “as well as” 
+“but also”, “however”, “whether”, “meanwhile”, “whereas”, “on the other hand”, or “otherwise”. 
+Examples:  
+Unacceptable: The user shall either be trusted or not trusted.  
+[This is unacceptable for several reasons.  The intention is that a user should be classified in 
+one of two ways, but it is also a passive requirement written on the user rather than on the 
+system (R2) and it is ambiguous: the requirement would still be met if the system took the 
+option of treating all users as trusted.] 
+Improved: The Security_System shall categorize each User as EITHER Trusted OR Not_Trusted. 
+Unacceptable:  The &lt;SOI&gt; shall display the Location and Identity of the Lead_Vehicle. 
+[This is unacceptable because is in fact stating two requirements which may well need to be 
+verified by different verification actions. In addition, the format of the displayed information is not 
+referenced.]  
+Improved: (Express as two requirements) 
+The &lt;SOI&gt; shall display the Location of the Lead_Vehicle per &lt;Display Standard xyx&gt;. 
+The &lt;SOI&gt; shall display the Identity of the Lead_Vehicle per &lt;Display Standard xyx&gt;. 
+Unacceptable:  The &lt;SOI&gt; shall provide an audible or visual alarm having the characteristics 
+defined in &lt;alarm standard xyz&gt;. 
+[This is unacceptable because it is a moot point as to whether the designer can choose which 
+alarm to implement, or (which is probably the intent of the writer) whether both alarms are 
+required, and the operator is alerted by at least one.]  
+Improved: (if the choice is available to the designer) 
+The &lt;SOI&gt; shall provide EITHER an Audible_Alarm OR Visual_Alarm having the 
+characteristics defined in &lt;Alarm Standard xyz&gt;. 
+Improved: (if both alarms are required) 
+_x000C_Guide to Writing Requirements 
+89 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+The &lt;SOI&gt; shall provide an Audible_Alarm having the characteristics defined in &lt;Alarm 
+Standard xyz&gt;. 
+The &lt;SOI&gt; shall provide a Visual_Alarm having the characteristics defined in &lt;Alarm Standard 
+xyz&gt;. 
+[As separate requirements, each can be allocated differently, and the SOI will be verified to 
+meet each. 
+Exceptions and relationships: 
+AND, OR, NOT can be used in need and requirement statements as logical conditions and 
+qualifiers as stated in R15. See also R16 and R17. 
+Combinators such as in “Command_and_Control” can be used in the project data dictionary, 
+ontology or glossary to cover one single function or quality of the system. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid phrases that indicate the “purpose of “, “intent of”, or “reason for” the need statement or 
+requirement statement. 
+Examples:  
+Unacceptable: The Record_Subsystem shall display the Name of each Line_Item so that the 
+Operator can confirm that it is the correct Item.   
+[This is unacceptable because the text “so that the Operator can confirm that it is the correct 
+Item” is rationale.] 
+Improved: The Record_Subsystem shall display the Name of each Line_Item per &lt;Display 
+Standard XYZ&gt;.   
+[The text “so that the Operator can confirm that it is the correct Item” should be included in the 
+rationale attribute.] 
+_x000C_Guide to Writing Requirements 
+90 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Unacceptable: The Operation_Logger shall record each Warning_Message produced by the 
+system.   
+[This is unacceptable because of the superfluous words “produced by the system”.] 
+Improved: The Operation_Logger shall record each Warning_Message within &lt;performance 
+measure&gt;. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid parentheses and brackets containing subordinate text. 
+Examples:  
+Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the 
+boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; 
+[This is unacceptable because of the parenthetical phrase as well as the ambiguous word 
+“usually”.   Note that the parameter Water_Temperature needs to be defined in the glossary in 
+order to be specific] 
+Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall 
+disconnect power from the Boiler within &lt;xxx ms&gt;. 
+[Note: for the above example, if this behavior is the result of a design decision, then the 
+requirement needs to be communicated as a design output.  The design input requirement 
+should focus on why this behavior is needed - for example, prevent the boiler from over 
+pressurizing and exploding. This is a good example of the benefit of asking “Why” for 
+requirements of this type.  The answer is the real design input requirement.   If included in the 
+set of Design Input Requirements, then the “why” should be included in the rationale.] 
+Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall 
+prevent the Boiler from over pressurization. 
+[How this is done is a design decision.} 
+Exceptions and relationships: 
+While this rule states brackets are to be avoided, R15 indicates that brackets may be used as 
+part of a convention for eliminating ambiguous conditions such as logical expressions. In that 
+case, it is useful to settle on a combination to be used—that is, for example, the organization 
+_x000C_Guide to Writing Requirements 
+91 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+template may avoid round brackets “(   )” in any statement and may use square brackets “[...]” in 
+logical expressions. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Enumerate sets explicitly instead of using a group noun to name the set. 
+Examples:  
+Unacceptable: The thermal control system shall manage temperature-related functions.   
+[This is unacceptable because there is ambiguity regarding which functions are to be managed 
+as well as what is meant by “managed”.  The specific functions should be enumerated explicitly 
+in separate requirement statements along with performance expectations and any applicable 
+conditions, triggers, or constraints.] 
+Unacceptable: The thermal control system shall monitor system temperature.   
+This is unacceptable because there is ambiguity regarding the function “monitor”.  Similar to 
+“managed” What are the expectations of the stakeholders – update the display of the system 
+temperature, maintain the temperature within some range, or store the history of the system 
+temperature? The specific subfunctions should be enumerated explicitly in separate 
+requirement statements along with performance expectations and any applicable conditions, 
+triggers, or constraints.] 
+Improved: (three separate requirements):  
+The Thermal_Control_System shall update the display of System_Temperature every 10 +/- 1 
+seconds. 
+The Thermal_Control_System shall maintain the System_Temperature between 95°C and 
+98°C.  
+The Thermal_Control_System shall store the history of System_Temperature.  
+[Note use of the glossary to define terms.] 
+Exceptions and relationships: 
+It is almost always better to enumerate members in a set, but the rule may be softened at the 
+higher levels of abstraction if the resulting requirement is sufficiently unambiguous.  For example, 
+at the business management level the business may state “ACME Consulting shall manage 
+_x000C_Guide to Writing Requirements 
+92 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Human Relations (HR) functions centrally.” or a system-level need statement may state: “The 
+&lt;stakeholders&gt; need the &lt;SOI&gt; to manage HR functions centrally.”  
+Although this raises the question of which HR functions are being referred to, it is not useful to 
+include a long list at these levels of abstractions and it is often not necessary since the statement 
+is sufficiently clear at the level at which it is stated.  The detailed enumeration of functions will be 
+undertaken at the business operations level, and the business management stakeholders should 
+be comfortable that no function will be omitted as a result of not listing it at the business 
+management level.   
+At the system level, need statements may include group nouns to name a set of entities or 
+include a higher-level function that is appropriate to the level of abstraction being communicated 
+within the need statement.  During the transformation of the need statement into requirements, 
+the project team would decompose the need into individual functional/performance requirements 
+as well as define requirements concerning the word “centrally” and would then validate with the 
+stakeholders that the resulting requirements, when realized, would meet the intent of the need 
+statement. 
+Another exemption would be to use the glossary or data dictionary to explicitly elaborate the set. 
+For example. “Account_Information” may be defined in the Glossary to include “Account_Name”, 
+“Account_Number”, and “Account_Balance”. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+When a need or requirement is related to complex behavior, refer to a supporting diagram, model, 
+or ICD. 
+Examples:  
+Unacceptable: The Control_System shall close Valves A AND B within 5 seconds of the 
+temperature exceeding 95 °C AND within 2 seconds of each other.   
+[This is unacceptable because of the confusing set of conditions.  In this case what is meant 
+will be clear if the requirement referred to a diagram for context.] 
+Improved: [Within 5 seconds of the temperature exceeding 95 °C] AND [within 2 seconds of each 
+other as shown in Timing_Diagram_6], the Control_System shall close [Valve A AND Valve B].   
+[Note that this assumes, of course, that the timing diagram itself is not ambiguous.  If it is not 
+possible to remove the ambiguity by using a diagram, it may be better to split the requirement 
+into two.] 
+[Note: for the above example, if this complex behavior is the result of a design decision, then 
+the requirement needs to be communicated as a design output.  The design input requirement 
+should focus on why this behavior is needed.] 
+Interface Example: 
+An interface requirement may refer to the characteristics of the electrical power (current/voltage) 
+being supplied by a system.   
+There can be multiple characteristics that need to be defined such that the systems receiving the 
+power have a clear understanding of the characteristics of the power they are receiving.  In this 
+case it is common for the characteristics to be defined in an ICD which both the provider and 
+receiver of the power can refer to in their Design Input Requirements.  From the provider 
+perspective the provider system will have to be verified that the power provided has all of these 
+characteristics and the receiver will have to verify it can receive and operate on power having 
+these same characteristics.   
+&lt;System 1&gt; shall provide power to &lt;System 2&gt; having the characteristics defined in &lt;ICD xyz&gt;. 
+Table 123&gt;. 
+&lt;System 2&gt; shall receive power from &lt;System 1&gt; having the characteristics defined in &lt;ICD 
+xyz&gt;. Table 123&gt;. 
+&lt;System 2&gt; shall operate on power having the characteristics defined in &lt;ICD xyz&gt;. Table 
+123&gt;. 
+4.5 Completeness 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the use of personal and indefinite pronouns. 
+Examples:  
+Unacceptable: The controller shall send the driver his itinerary for the day. It shall be delivered at 
+least 8 hours prior to his Shift.  
+[This is unacceptable because the requirement is expressed as two sentences and the second 
+sentence uses the pronouns “it” and “his.”] 
+Improved: At least 8 hours prior to the Driver_Shift, the Controller shall send the Driver_Itinerary 
+for the day to the Driver.   
+[Note use of the glossary to define terms and to be explicit about the relationship between the 
+driver, shift, and the itinerary for that particular driver.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid relying on headings to support explanation or understanding of the need or requirement. 
+Examples:  
+Example heading: “4.0 Alert Buzzer Requirements.”  
+Unacceptable: 4.1 The &lt;SOI&gt; shall sound it for greater than 20 minutes.   
+[This is unacceptable because the requirement uses the pronoun “it” (R24), which requires the 
+heading to understand what “it” means.  In addition, the word “sound” could be ambiguous as it 
+can be a noun, a verb, adverb, or adjective.  We do not know whether Alert_Buzzer is a 
+subsystem that controls the noise or the thing that makes the noise.] 
+Improved: When &lt;triggering event&gt;, the &lt;SOI&gt; shall sound an alert having the characteristics 
+defined in &lt;Alert Standard xyz&gt; for greater than 20 minutes. 
+[In this improved rewrite, the existence of the header is not needed to interpret the requirement.  
+Even though the above heading referenced an “Alert Buzzer”—an implementation, the improved 
+requirement avoids implementation to a specific device, and rather indicates that when the 
+triggering event happens, an alert is required to be sounded having the characteristics defined in 
+the alert standard. 
+Exceptions and relationships: 
+The use of headings is useful and acceptable when producing an output of an RMT, grouping like 
+types or categories of needs or requirements.  However, care must be taken that the headings 
+are used solely for management of the subsets of statements—the heading must not be 
+necessary to understand any of the grouped statements. See R41 and R42. 
+4.6 Realism 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid using unachievable absolutes. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall have 100% availability.   
+[This is unacceptable because 100% is an absolute that is impossible to achieve and verify.  
+Also, available over what time period?] 
+Improved: The &lt;SOI&gt; shall have an Availability of greater than or equal to 98% during 
+Operating_Hours. 
+[Note use of the glossary to define Operating_Hours. Alternatively, this requirement could be 
+stated as a need.  Then those transforming the need into requirements would develop a 
+_x000C_Guide to Writing Requirements 
+96 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+feasible concept for doing so and then derive specific Design Input Requirements that would 
+result in the need being met.] 
+Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 
+30 minutes.   
+[This is unacceptable because the requirement is impossibly precise to maintain in terms of the 
+flow rate (and impossibly precise to measure in verification) as well as being impossibly precise 
+to deliver for 30 minutes exactly. Also, it is not clear under what conditions this applies—when in 
+operations, when powered on, when commanded?] 
+Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters 
+per second for greater than 30 minutes.   
+[Now the range of acceptable flow performance and time frame is clear and feasible.  Given that 
+the condition “when in operations” this requirement applies whenever the Pumping_Station is 
+active—no matter how long. Also, what is the intent for how long—31 minutes satisfies the 
+requirement, but what if the real intent is for however long the Pumping Station is in operations 
+which could be hours or days—again depending on the operating conditions and need. Further, 
+is the 30 minutes of continuous flow or a total of 30 minutes within a set time period?] 
+4.7 Conditions 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+State conditions’ applicability explicitly instead of leaving applicability to be inferred from the 
+context. 
+Examples:  
+Unacceptable:  
+The Free_Access_Mode shall be set to ON within &lt;xxx ms&gt;. 
+The Fire_Door_Unlock command having the characteristics defined in &lt;ICD xyz&gt; shall be 
+sent to each Fire_Door within &lt;xxx ms&gt;. 
+[This is unacceptable because the condition or trigger for these actions is not stated. Also, note 
+the actions are written in passive voice which violates R2.  Each action needs to be 
+communicated in a separate active voice requirement statement with the condition or trigger for 
+which the action is to be initiated.  For multiple conditions for a single action see R28.] 
+Improved: (Split into two requirements) 
+In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode 
+to ON within &lt;xxx ms&gt;. 
+In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock 
+unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within 
+&lt;xxx ms&gt;. 
+[Note that there is a Fire Detection subsystem responsible for detecting fires and setting the 
+Fire_Detection parameter to “TRUE” which triggers the two actions.   All other subsystems that 
+are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” will 
+have their own requirements to monitor this parameter and take the required action(s) as stated 
+in their set of requirements.  All Fire Doors will have their own requirements to monitor for the 
+Fire_Door_Unlock command and to unlock when the command is received.] 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Express the propositional nature of a condition explicitly for a single action instead of giving lists of 
+actions for a specific condition. 
+Examples:  
+_x000C_Guide to Writing Requirements 
+98 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Unacceptable:  
+The Audit _Clerk shall be able to change the status of the action item when: 
+ - the Audit _Clerk originated the item; 
+ - the Audit _Clerk is the actionee; and 
+ - the Audit _Clerk is the reviewer. 
+[This is unacceptable because it is not clear whether all the conditions must hold (a 
+conjunction) or any one of them (a disjunction).  Also, the requirement contains the phrase “be 
+able to” which violates R11.] 
+Better: If the requirement is interpreted as a disjunction:  
+The Audit_System shall change the Action_Item status requested by the Audit_Clerk when one 
+or more of the following conditions are true: 
+ - the Audit_Clerk originated the Action_Item; 
+ - the Audit_Clerk is the Actionee; or 
+ - the Audit_Clerk is the Reviewer. 
+[Although the requirement is now improved, there is still the issue of verification. If the status 
+does not change with one of the listed conditions, then the entire requirement fails verification, 
+even if the other two conditions are met as specified.] 
+Better: In this case, it would be best to state three distinct requirements as this makes each 
+atomic and retains the same overall intent.  From an allocation, traceability, and verifiability 
+perspective this form is preferable. 
+The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
+Audit_Clerk originated the Action_Item. 
+The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
+Audit_Clerk is the Actionee. 
+The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
+Audit_Clerk is the Reviewer. 
+Better if interpreted as a conjunction:  
+The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the 
+following conditions are true: 
+ - the Audit_Clerk originated the Action_Item AND 
+ - the Audit_Clerk is the Actionee AND 
+ - the Audit_Clerk is the Reviewer. 
+[In this form, the three conditions are expressed as a logical condition such that all three must 
+all be true for the logical condition to be true.] 
+4.8 Uniqueness 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Classify needs and requirements according to the aspects of the problem or system it addresses. 
+Examples:  
+Example classifications: Functional, Performance, Operational, Reliability, Availability, 
+Maintainability, Safety, Security, Design and Construction Standards, Physical Characteristics.  
+See the NRM for more guidance on organizing needs and requirements. 
+See Also R41 – Related Requirements 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Express each need and requirement once and only once. 
+Examples:  
+Exact duplicates can be found by matching of text strings.  The main problem is to identify 
+similarities with different expressions, but which are equivalent.   
+For example, the following statements are overlapping in that the first is a subset of the second: 
+The &lt;SOI &gt; shall generate a report of financial transactions containing the information defined in 
+&lt;some standard or contract deliverable listing&gt;. 
+The &lt;SOI&gt; shall generate a financial report. 
+4.9 Abstraction 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid stating implementation in a need statement or requirement statement unless there is 
+rationale for constraining the design. 
+Examples:  
+General: For a medical diagnostic system 
+• Stakeholders need statement: “The &lt;stakeholders&gt; need the &lt;diagnostic system&gt; to measure 
+[something] with an accuracy as good as or better than similar devices in the market.”  
+[This is an appropriate level of abstraction for a stakeholder need statement, clearly stating 
+the expectation the stakeholders have concerning accuracy, however this would not be a 
+good design input requirement.] 
+• Requirement transformed from the stakeholder need statement: “The &lt;diagnostic system&gt; 
+shall measure [something] with an accuracy of [xxx].”  
+[The developers have explored various concepts for meeting the need for accuracy, have 
+examined candidate technologies, have accessed their maturity (technology readiness level 
+(TRL), and have decided that the value [xxx] is feasible with acceptable risk for this lifecycle 
+stage.  As stated, this is an appropriate level of detail for a design input requirement.] 
+Note that when dealing with measures, both accuracy and precision must be addressed, either 
+as separate requirements or including both in a measurement requirement defining 
+characteristics of the measured parameter. 
+These system-level design input accuracy and precision requirements are then allocated to the 
+parts of the system architecture that have a role in meeting the overall system accuracy and 
+precision requirements.  For a medical diagnostic system this could include allocations to the 
+hardware (instrument), assay (biological sample), and software.  These allocations could then 
+be further sub-allocated within the hardware, assay, and software lower-level entities.   
+As long as the requirements are written on the accuracy and precision allocations and not how 
+that accuracy or precision will be obtained by one of the architectural entities, the requirements 
+are Design Input Requirements.  As soon as specific hardware components are named (laser, 
+LEDs emitting light at a specific wavelength, optical system components, specific 
+magnifications, algorithms, formulations, etc.,) then the requirements are reflecting design 
+outputs and need to be communicated within design output artifacts (specifications).  
+Unacceptable: Traffic lights shall be used to control traffic at the intersection.   
+[This is unacceptable because “Traffic lights” are a solution (design output).  Why are traffic 
+lights needed? This requirement is also written in passive voice - see R2] 
+Improved: (several requirements): 
+When a Pedestrian signals an intent to cross the street at the Intersection, the 
+Traffic_Control_System shall provide [the Pedestrian a “Walk” signal AND provide the traffic a 
+“Stop” signal]. 
+The Traffic_Control_System shall limit the Wait_Time of Vehicles traversing the Intersection to 
+less than Daylight_Wait_Time during Normal_Daytime traffic conditions.   
+[Note that glossary definitions should be used for Traffic_Control_System, 
+Daylight_Wait_Time_Value, Normal_Daytime, Vehicles, and Intersection.] 
+Unacceptable: When a pedestrian signals his presence by pressing a button on the traffic-light 
+pillar, the traffic light shall turn red for the traffic to stop.   
+[This is unacceptable because this requirement contains solution-biased detail - design output.  
+In addition, the requirement is unacceptable because it has additional information concerning 
+_x000C_Guide to Writing Requirements 
+102 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+the action traffic is to take and does not specify the duration of the red light.  The use of a 
+pronoun is also not recommended]. 
+Improved: When the presence of a Pedestrian that needs to cross the street at the Intersection 
+during Day_Light_Hours is detected, the Traffic_Control_System shall issue a 
+Traffic_Stop_Signal for Average_Pedestrian_Crossing_Time.  
+[This design input requirement allows freedom in determining the best solution (design output), 
+which may be a means of automatic detection rather than button pushing along with the type 
+and characteristics of the signal issued.  Note that pedestrians may be in proximity of the 
+intersection that do not wish to cross the street.]  
+[An interesting consideration from a consistency or conflict perspective, what if the 
+Average_Pedestrian_Crossing_Time” is greater than the “Daylight_Wait_Time_Value” defined 
+for the traffic in the previous example.  Each time is from a different entity perspective.] 
+[Note that glossary definitions should be used for “Pedestrian”, “Traffic_Control_System”, 
+“Traffic_Stop_Signal”, “Day_Light_Hours”, “Average_Pedestrian_Crossing_Time”, and 
+“Intersection”.] 
+Exceptions and relationships: 
+Sometimes solutions have to be described in requirements, even if it is very detailed for a given 
+level, for example if the airworthiness authorities require the use of a specific template for a 
+certain report; or if a naval customer requires that the new naval vessel be equipped with a 
+specific weapon system from a specific supplier; or if all vehicles in a fleet are required to use the 
+same fuel or the next model make use of a particular engine. In these cases, it is not a premature 
+solution, but a real stakeholder or customer need concerning a constraint.  As such this is 
+acceptable as a design input. 
+However, as a rule, if a detailed, specific design solution is expressed as a design input without 
+proper justification, it may be a premature solution and should be communicated as a design 
+output and an appropriate set of design input needs and associated requirements developed that 
+communicate “For what purpose?” which the design output requirements can be traced to.  
+Examples of issues concerning design outputs expressed as design inputs include: 
+1. The project is developing an upgrade to an existing system (brownfield SE).  Rather than 
+documenting design input “what” requirements, the project team focuses on known solutions 
+and implementations and documenting design output level requirements as design inputs.  
+This is problematic in that the real “for what purpose?” question is not being addressed and 
+the real Design Input Requirements are not communicated. 
+2. A similar case exists when procuring an off-the-shelf (OTS) solution and communicating the 
+requirements for that solution as Design Input Requirements rather than in a design output 
+specification.  Again, this is problematic in that the real “for what purpose?” question is not 
+being addressed and the real Design Input Requirements are not communicated. 
+3. A common issue arises when an existing system or OTS exists, yet the project develops 
+and documents as design inputs a detailed design output level set of requirements (design 
+output specification) for the system rather than a set of design input set of “what” 
+requirements that would guide the selection of an appropriate OTS.  This can result in a 
+redundant set of requirements that are not necessary, will have to be verified - adding 
+additional cost to the project, yet not addressing the “for what purpose?” design input 
+requirement set that should drive the selection of the specific OTS.  Refer to the NRM for a 
+detailed discussion the use of OTS entities. 
+_x000C_Guide to Writing Requirements 
+103 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+4. As part of the lifecycle concept analysis and maturation activities the project team developed 
+a prototype to access feasibility.  The resulting needs and resulting requirements are based 
+on the prototype and an associated trade study that resulted a specific solution that meets 
+the needs of the stakeholders.  Rather than communicating the Design Input Requirements, 
+the design output requirements for the prototype are included in the design input set of 
+requirements while not addressing the “for what purpose?” design input requirement set that 
+would drive the design for the prototype. 
+4.10 Quantifiers 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use “each” instead of “all”, “any”, or “both” when universal quantification is intended. 
+Examples:  
+Unacceptable: The Operation_Logger shall record any (or all) warning messages.   
+[This is unacceptable because of the use of the word “any”, which is then made worse by the 
+addition of “(or all)”.] 
+Improved: The Operation_Logger shall record each Warning_Message.   
+[Note that Warning_Message must be defined in the glossary so that it is clear that the SOI only 
+will record each defined Warning Message. Also, any conditions or performance must also be 
+included in the requirements statement for it to be complete.] 
+Unacceptable: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Names of 
+both of the Line_Items.   
+[This is unacceptable because of the use of the word “both”.] 
+Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Name of each 
+Line_Item.  
+Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; each 
+Line_Item_Name. 
+4.11 Tolerance 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Define each quantity with a range of values appropriate to the entity to which the quantity applies 
+and against which the entity will be verified or validated. 
+_x000C_Guide to Writing Requirements 
+104 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Examples:  
+Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 
+30 minutes.   
+[This is unacceptable because we do not know whether a solution that addresses more or less 
+than the specified quantities is acceptable Also, it is not clear under what conditions this applies 
+– when in operations, when powered on, when commanded?] 
+Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters 
+for a minimum of 30 minutes.   
+[Now the range of acceptable flow performance is clear and that the 30 minutes is a minimum 
+acceptable performance.  Given that the condition “when in operations”, this requirement applies 
+whenever the Pumping_Station is active—no matter how long. Also, a question to be asked is 
+what is the intent for how long—31 minutes satisfies the requirement, but what if the real intent is 
+for however long the Pumping Station is in operations which could be hours or days – again 
+depending on the operating conditions and need. What if there is not enough water at the inlet to 
+the pumping station to establish the required flow rate?] 
+Unacceptable: The Flight_Information_System shall display the current altitude to approximately 
+1 meter resolution.   
+[This is unacceptable because it is imprecise.  What is “approximately” in the context of a 
+distance of 1 meter?  Who has the option of deciding what is “approximately”?  How will 
+“approximately” be verified?  What is the acceptable tolerance?]  
+[Note that care must be taken to confirm that the units are appropriate in the context of the 
+organizational and project templates.  See also R6.] 
+Improved: The Flight_Information_System shall display Current_Altitude with an accuracy of ±1 
+meter.   
+[Note that “Current_Altitude” must be defined in the glossary since there are a number of 
+possible interpretations of the term.] 
+Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to allowable 
+levels.  Rationale: Arsenic contamination in drinking water can cause health problems.   
+[While “allowable” is acceptable in a need statement, it is unacceptable in a requirement 
+statement because allowable is ambiguous - allowable by whom?  What specific concentration 
+is allowable?  In what market?] 
+Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to 1 part per 
+trillion.  Rationale Attribute (A1): Arsenic contamination in drinking water can cause health 
+problems.   
+[This is unacceptable because the EPA contamination limit in drinking water is 10 parts per 
+billion.  Requiring a tighter limit may be beyond the ability of current technology to measure or 
+if measuring concentrations of 1 part per trillion are possible, the cost to do so may be 
+unacceptably high.  Also, no range is specified.  Using ‘less than’ is probably the real intent.] 
+Improved: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to less than10 parts 
+per billion.  Rationale Attribute (A1): EPA set the arsenic standard for drinking water at 10 ppb (or 
+0.010 parts per million).  The EPA has determined that concentrations of this level or less will 
+protect consumers from the effects of long-term, chronic exposure to arsenic. 
+Exceptions and relationships: 
+_x000C_Guide to Writing Requirements 
+106 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+The use of tolerances in need statements may not be as mandatory as their use in requirement 
+statements—see Appendix D. 
+4.12 Quantification 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Provide specific measurable performance targets appropriate to the entity to which the need or 
+requirement is stated and against which the entity will be verified to meet. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall use minimum power.   
+[This is unacceptable because both words “use” and “minimum” are ambiguous and 
+unverifiable.] 
+Improved: The &lt;SOI&gt; shall consume less than or equal to 50W of mains power.   
+[This both considers the underlying goal—to minimize power consumption—and provides a 
+measurable target.] 
+Unacceptable: The engine shall achieve an emissions level that is at least 5% less than the 
+competition’s emission levels 2 years from now.   
+[This is an actual requirement from marketing to an engineering department.  The statement 
+sets a completely unmeasurable end state.] 
+Improved: The Engine shall achieve an emissions level that is less than or equal to xxx.   
+[where xxx represents the required threshold value, including the appropriate units.] 
+Unacceptable: The &lt;SOI&gt; shall conform to best practices for spurious emissions. 
+[This statement is vague and unverifiable from number of specifics] 
+Improved: The &lt;SOI&gt; shall limit Spurious_Emissions in accordance with &lt;Clause xab of Standard 
+XYZ&gt;. 
+Exceptions and relationships: 
+Some quantification terms such as “minimum”, “maximum”, “optimal” are almost always 
+ambiguous.  Other terms may be ambiguous at lower levels but sufficient at the higher levels and 
+as need statements.  For example, it may be appropriate that the business state that “The Aircraft 
+shall provide class-leading comfort.”—while such a requirement is not quantifiable and therefore 
+not measurable, it may be sufficient for the business to communicate its intentions as a need 
+_x000C_Guide to Writing Requirements 
+107 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+statement to developers who can then turn comfort into such measurable quantities such as seat 
+dimensions and leg length.  
+This exception also applies to needs stated at the system or system element levels. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Define temporal dependencies explicitly instead of using indefinite temporal keywords such as 
+“eventually”, “until”, “before”, “after”, “as”, “once”, “earliest”, “latest”, “instantaneous”, 
+“simultaneous”, and “at last”. 
+Examples:  
+Unacceptable: Continual operation of the pump shall eventually result in the tank being empty.   
+[This is unacceptable because “eventually” is ambiguous.  Also, this statement is not written in 
+the proper form.  It is written on “operation” rather than on a requirement on the pump which 
+violates R3.] 
+Improved: The Pump shall remove greater than 99% of the Fluid from the Tank in less than 3 
+days of continuous operation. 
+4.13 Uniformity of Language 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use each term and unit of measure consistently throughout need and requirement sets as well as 
+associated models and other SE artefacts developed across the lifecycle. 
+Examples:  
+Unacceptable: It would not be acceptable for one requirement to refer to an entity using one term 
+and another to refer to the same entity using another term. 
+For example, a subsystem set of Design Input Requirements contains the following three 
+requirement statements: 
+    The Radio shall ....  
+    The Receiver shall .... 
+    The Terminal shall .... 
+Or: 
+    The Bleed_Valve shall ....  
+    The High-Pressure_Bleed_Valve shall .... 
+    The HPBV shall .... 
+If each term refers to the same subject, the statements need to be modified to use the same word 
+(or, if they are meant to be different, the words must be defined to be so). 
+Improved: Settle on only one term, define it in the glossary or data dictionary, and then use it 
+consistently in each need, requirement, and design output artifact. 
+Unacceptable: When the Input_Valve is connected to the Water_Source, the Control_Subsystem 
+shall open the Inlet_Valve.   
+[Two terms are used for the same thing “Input_Valve” and “Inlet_Valve”.] 
+Improved: When the Inlet_Valve is connected to the Water_Source, the Control_Subsystem shall 
+open the Inlet_Valve. 
+Unacceptable: It would not be acceptable for one requirement to use one unit of measure (for 
+example, US - feet) and another requirement to use another unit of measure (for example, Metric 
+- meter). 
+_x000C_Guide to Writing Requirements 
+109 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Improved: Settle on which units of measure will be used and use that unit of measure consistency 
+across all SE artifacts including needs, Design Input Requirements and design output 
+specifications.  
+Also, see R40 for guidance regarding the conversion from one measurement system to another 
+and the use of significant digits. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+If acronyms are used, they must be consistent throughout need and requirement sets as well as 
+associated models and other SE artefacts developed across the lifecycle. 
+Examples:  
+Unacceptable: It would not be acceptable for one requirement to use the acronym “CP” for 
+command post and another acronym “CMDP” to also refer to the “command post.” The use of two 
+different acronyms implies that the two system elements being referred to are different. 
+Improved: Settle on only one acronym, define it in the list of acronyms, and then use it 
+consistently throughout the requirement set. 
+Unacceptable: It would not be acceptable for one requirement to refer to the “Global Positioning 
+System” and the remaining requirements refer just to “GPS.” 
+Improved: Use the full term every time or, perhaps more usefully, define the acronym in the 
+project acronym list or glossary and use it every time. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Avoid the use of abbreviations in needs and requirement statements as well as associated 
+models and other SE lifecycle artefacts. 
+_x000C_Guide to Writing Requirements 
+110 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Examples:  
+Unacceptable: It would not be acceptable for one requirement to refer to the abbreviation “op” 
+meaning operation and another to refer to the “op” meaning the operator. 
+Improved: Avoid the abbreviation and use the full term every time. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use a project-wide style guide for individual need statements and requirement statements. 
+Examples:  
+For example, each organization should have a style guide or schema to address such issues as 
+the selection and definition of what need patterns and requirement patterns should be used for 
+writing need statements and requirement statements of a particular type, the selection and use of 
+attributes, standard abbreviations and acronyms, layout and use of figures and tables, layout of 
+documents or databases and, statement numbering.  
+_x000C_Guide to Writing Requirements 
+111 
+INCOSE-TP-2010-006-04| VERS/REV:4  |  1 July 2023 
+Terms used throughout the sets of needs and sets of requirements are defined in an ontology or 
+at least a project glossary. 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Use a consistent format and number of signification digits for the specification of decimal 
+numbers. 
+Examples:  
+Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp;  
+The &lt;SOI&gt; shall consume less than or equal to 0.99 W. 
+[These two statements are unacceptable when included in the same set because a different 
+format is used in the two statements.] 
+Improved:  
+The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp;  
+The &lt;SOI&gt; shall consume less than or equal to 0.99 W.  
+OR  
+The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp;  
+The &lt;SOI&gt; shall consume less than or equal to 0,99 W. 
+Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 0.99 h. &amp;  
+The &lt;SOI&gt; shall consume less than or equal to .99 W. 
+[These two statements are unacceptable when included in the same set because a different 
+format is used in the two statements.] 
+Improved:  
+The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp;  
+The &lt;SOI&gt; shall consume less than or equal to 0.99 W.  
+4.14 Modularity 
+4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:  
+Group related needs and requirements together. 
+Examples:  
+Requirements may be related by: 
+- type (for example, critical functions, enabling functions, safety, or security requirements); 
+- scenario (for example, requirements arising from a single scenario). 
+- interactions with other systems (for example interface requirements). 
+- function (for example, multiple requirements defined for a function, each addressing a different 
+performance characteristics, mode, state, condition, or trigger.) 
+- capability (for example a needed capability may be released by a set of requirements that 
+together result in the needed capability to be provided. 
+-compliance (for example requirements whose purpose it is to implement a requirement in a 
+standard or regulation. 
+See R29 and the NRM for more guidance on organizing needs and requirements. 
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:  
+Conform to a defined structure or template for organizing sets of needs and requirements. 
+Examples:  
 For sets of needs or requirements, an outline can be defined that organizes them in categories or 
 by type.   
 Examples of Type/Category of needs and requirements include:  
@@ -5419,13 +6832,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5456,8 +6869,20 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5468,10 +6893,10 @@
         <v>1890</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F2">
         <v>1890</v>
@@ -5480,19 +6905,31 @@
         <v>3631</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="J2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="K2" t="s">
-        <v>220</v>
+        <v>224</v>
+      </c>
+      <c r="L2" t="s">
+        <v>266</v>
+      </c>
+      <c r="M2" t="s">
+        <v>267</v>
+      </c>
+      <c r="N2" t="s">
+        <v>266</v>
+      </c>
+      <c r="O2" t="s">
+        <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5503,10 +6940,10 @@
         <v>3636</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F3">
         <v>3636</v>
@@ -5515,19 +6952,31 @@
         <v>7472</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="J3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="K3" t="s">
-        <v>221</v>
+        <v>225</v>
+      </c>
+      <c r="L3" t="s">
+        <v>266</v>
+      </c>
+      <c r="M3" t="s">
+        <v>267</v>
+      </c>
+      <c r="N3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O3" t="s">
+        <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5538,10 +6987,10 @@
         <v>7477</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F4">
         <v>7477</v>
@@ -5550,19 +6999,31 @@
         <v>16353</v>
       </c>
       <c r="H4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="J4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="K4" t="s">
-        <v>222</v>
+        <v>226</v>
+      </c>
+      <c r="L4" t="s">
+        <v>266</v>
+      </c>
+      <c r="M4" t="s">
+        <v>267</v>
+      </c>
+      <c r="N4" t="s">
+        <v>266</v>
+      </c>
+      <c r="O4" t="s">
+        <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5573,10 +7034,10 @@
         <v>16358</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F5">
         <v>16358</v>
@@ -5585,19 +7046,31 @@
         <v>20821</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I5" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="J5" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="K5" t="s">
-        <v>223</v>
+        <v>227</v>
+      </c>
+      <c r="L5" t="s">
+        <v>266</v>
+      </c>
+      <c r="M5" t="s">
+        <v>267</v>
+      </c>
+      <c r="N5" t="s">
+        <v>266</v>
+      </c>
+      <c r="O5" t="s">
+        <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5608,10 +7081,10 @@
         <v>20826</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F6">
         <v>20826</v>
@@ -5620,19 +7093,31 @@
         <v>24520</v>
       </c>
       <c r="H6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="J6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="K6" t="s">
-        <v>224</v>
+        <v>228</v>
+      </c>
+      <c r="L6" t="s">
+        <v>266</v>
+      </c>
+      <c r="M6" t="s">
+        <v>267</v>
+      </c>
+      <c r="N6" t="s">
+        <v>266</v>
+      </c>
+      <c r="O6" t="s">
+        <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5643,10 +7128,10 @@
         <v>24525</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F7">
         <v>24525</v>
@@ -5655,19 +7140,31 @@
         <v>29695</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I7" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="J7" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="K7" t="s">
-        <v>225</v>
+        <v>229</v>
+      </c>
+      <c r="L7" t="s">
+        <v>266</v>
+      </c>
+      <c r="M7" t="s">
+        <v>267</v>
+      </c>
+      <c r="N7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O7" t="s">
+        <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5678,10 +7175,10 @@
         <v>29700</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <v>29700</v>
@@ -5690,19 +7187,31 @@
         <v>33100</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="K8" t="s">
-        <v>226</v>
+        <v>230</v>
+      </c>
+      <c r="L8" t="s">
+        <v>266</v>
+      </c>
+      <c r="M8" t="s">
+        <v>267</v>
+      </c>
+      <c r="N8" t="s">
+        <v>266</v>
+      </c>
+      <c r="O8" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5713,10 +7222,10 @@
         <v>33105</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F9">
         <v>33105</v>
@@ -5725,19 +7234,31 @@
         <v>34958</v>
       </c>
       <c r="H9" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="K9" t="s">
-        <v>227</v>
+        <v>231</v>
+      </c>
+      <c r="L9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M9" t="s">
+        <v>267</v>
+      </c>
+      <c r="N9" t="s">
+        <v>266</v>
+      </c>
+      <c r="O9" t="s">
+        <v>275</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5748,10 +7269,10 @@
         <v>34963</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F10">
         <v>34963</v>
@@ -5760,19 +7281,31 @@
         <v>37730</v>
       </c>
       <c r="H10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I10" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="J10" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="K10" t="s">
-        <v>228</v>
+        <v>232</v>
+      </c>
+      <c r="L10" t="s">
+        <v>266</v>
+      </c>
+      <c r="M10" t="s">
+        <v>267</v>
+      </c>
+      <c r="N10" t="s">
+        <v>266</v>
+      </c>
+      <c r="O10" t="s">
+        <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5783,10 +7316,10 @@
         <v>37735</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F11">
         <v>37735</v>
@@ -5795,19 +7328,31 @@
         <v>42493</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I11" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="J11" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="K11" t="s">
-        <v>229</v>
+        <v>233</v>
+      </c>
+      <c r="L11" t="s">
+        <v>266</v>
+      </c>
+      <c r="M11" t="s">
+        <v>267</v>
+      </c>
+      <c r="N11" t="s">
+        <v>266</v>
+      </c>
+      <c r="O11" t="s">
+        <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5818,10 +7363,10 @@
         <v>42498</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F12">
         <v>42498</v>
@@ -5830,19 +7375,31 @@
         <v>44938</v>
       </c>
       <c r="H12" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K12" t="s">
-        <v>230</v>
+        <v>234</v>
+      </c>
+      <c r="L12" t="s">
+        <v>266</v>
+      </c>
+      <c r="M12" t="s">
+        <v>267</v>
+      </c>
+      <c r="N12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O12" t="s">
+        <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5853,10 +7410,10 @@
         <v>44943</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <v>44943</v>
@@ -5865,19 +7422,31 @@
         <v>49509</v>
       </c>
       <c r="H13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="J13" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="K13" t="s">
-        <v>231</v>
+        <v>235</v>
+      </c>
+      <c r="L13" t="s">
+        <v>266</v>
+      </c>
+      <c r="M13" t="s">
+        <v>267</v>
+      </c>
+      <c r="N13" t="s">
+        <v>266</v>
+      </c>
+      <c r="O13" t="s">
+        <v>279</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5888,10 +7457,10 @@
         <v>49514</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F14">
         <v>49514</v>
@@ -5900,19 +7469,31 @@
         <v>53099</v>
       </c>
       <c r="H14" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="I14" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="J14" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="K14" t="s">
-        <v>232</v>
+        <v>236</v>
+      </c>
+      <c r="L14" t="s">
+        <v>266</v>
+      </c>
+      <c r="M14" t="s">
+        <v>267</v>
+      </c>
+      <c r="N14" t="s">
+        <v>266</v>
+      </c>
+      <c r="O14" t="s">
+        <v>280</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5923,10 +7504,10 @@
         <v>53104</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F15">
         <v>53104</v>
@@ -5935,19 +7516,31 @@
         <v>55211</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="I15" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="J15" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="K15" t="s">
-        <v>233</v>
+        <v>237</v>
+      </c>
+      <c r="L15" t="s">
+        <v>266</v>
+      </c>
+      <c r="M15" t="s">
+        <v>267</v>
+      </c>
+      <c r="N15" t="s">
+        <v>266</v>
+      </c>
+      <c r="O15" t="s">
+        <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5958,10 +7551,10 @@
         <v>55216</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F16">
         <v>55216</v>
@@ -5970,19 +7563,31 @@
         <v>58295</v>
       </c>
       <c r="H16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I16" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="J16" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="K16" t="s">
-        <v>234</v>
+        <v>238</v>
+      </c>
+      <c r="L16" t="s">
+        <v>266</v>
+      </c>
+      <c r="M16" t="s">
+        <v>267</v>
+      </c>
+      <c r="N16" t="s">
+        <v>266</v>
+      </c>
+      <c r="O16" t="s">
+        <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:15">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5993,10 +7598,10 @@
         <v>58300</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F17">
         <v>58300</v>
@@ -6005,19 +7610,31 @@
         <v>61219</v>
       </c>
       <c r="H17" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I17" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="J17" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="K17" t="s">
-        <v>235</v>
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>266</v>
+      </c>
+      <c r="M17" t="s">
+        <v>267</v>
+      </c>
+      <c r="N17" t="s">
+        <v>266</v>
+      </c>
+      <c r="O17" t="s">
+        <v>283</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6028,10 +7645,10 @@
         <v>61224</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F18">
         <v>61224</v>
@@ -6040,19 +7657,31 @@
         <v>63959</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="J18" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K18" t="s">
-        <v>236</v>
+        <v>240</v>
+      </c>
+      <c r="L18" t="s">
+        <v>266</v>
+      </c>
+      <c r="M18" t="s">
+        <v>267</v>
+      </c>
+      <c r="N18" t="s">
+        <v>266</v>
+      </c>
+      <c r="O18" t="s">
+        <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:15">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6063,10 +7692,10 @@
         <v>63964</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F19">
         <v>63964</v>
@@ -6075,19 +7704,31 @@
         <v>72805</v>
       </c>
       <c r="H19" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I19" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="J19" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K19" t="s">
-        <v>237</v>
+        <v>241</v>
+      </c>
+      <c r="L19" t="s">
+        <v>266</v>
+      </c>
+      <c r="M19" t="s">
+        <v>267</v>
+      </c>
+      <c r="N19" t="s">
+        <v>266</v>
+      </c>
+      <c r="O19" t="s">
+        <v>285</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:15">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -6098,10 +7739,10 @@
         <v>72810</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F20">
         <v>72810</v>
@@ -6110,19 +7751,31 @@
         <v>75754</v>
       </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I20" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="J20" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="K20" t="s">
-        <v>238</v>
+        <v>242</v>
+      </c>
+      <c r="L20" t="s">
+        <v>266</v>
+      </c>
+      <c r="M20" t="s">
+        <v>267</v>
+      </c>
+      <c r="N20" t="s">
+        <v>266</v>
+      </c>
+      <c r="O20" t="s">
+        <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:15">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -6133,10 +7786,10 @@
         <v>75759</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F21">
         <v>75759</v>
@@ -6145,19 +7798,31 @@
         <v>78047</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I21" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="J21" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K21" t="s">
-        <v>239</v>
+        <v>243</v>
+      </c>
+      <c r="L21" t="s">
+        <v>266</v>
+      </c>
+      <c r="M21" t="s">
+        <v>267</v>
+      </c>
+      <c r="N21" t="s">
+        <v>266</v>
+      </c>
+      <c r="O21" t="s">
+        <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:15">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6168,10 +7833,10 @@
         <v>78052</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F22">
         <v>78052</v>
@@ -6180,19 +7845,31 @@
         <v>80665</v>
       </c>
       <c r="H22" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I22" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="J22" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="K22" t="s">
-        <v>240</v>
+        <v>244</v>
+      </c>
+      <c r="L22" t="s">
+        <v>266</v>
+      </c>
+      <c r="M22" t="s">
+        <v>267</v>
+      </c>
+      <c r="N22" t="s">
+        <v>266</v>
+      </c>
+      <c r="O22" t="s">
+        <v>288</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:15">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -6203,10 +7880,10 @@
         <v>80670</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F23">
         <v>80670</v>
@@ -6215,19 +7892,31 @@
         <v>84721</v>
       </c>
       <c r="H23" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I23" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="J23" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="K23" t="s">
-        <v>241</v>
+        <v>245</v>
+      </c>
+      <c r="L23" t="s">
+        <v>266</v>
+      </c>
+      <c r="M23" t="s">
+        <v>267</v>
+      </c>
+      <c r="N23" t="s">
+        <v>266</v>
+      </c>
+      <c r="O23" t="s">
+        <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -6238,10 +7927,10 @@
         <v>84726</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F24">
         <v>84726</v>
@@ -6250,19 +7939,31 @@
         <v>88927</v>
       </c>
       <c r="H24" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="I24" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="J24" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="K24" t="s">
-        <v>242</v>
+        <v>246</v>
+      </c>
+      <c r="L24" t="s">
+        <v>266</v>
+      </c>
+      <c r="M24" t="s">
+        <v>267</v>
+      </c>
+      <c r="N24" t="s">
+        <v>266</v>
+      </c>
+      <c r="O24" t="s">
+        <v>290</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:15">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -6273,10 +7974,10 @@
         <v>88932</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F25">
         <v>88932</v>
@@ -6285,19 +7986,31 @@
         <v>91525</v>
       </c>
       <c r="H25" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I25" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="J25" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="K25" t="s">
-        <v>243</v>
+        <v>247</v>
+      </c>
+      <c r="L25" t="s">
+        <v>266</v>
+      </c>
+      <c r="M25" t="s">
+        <v>267</v>
+      </c>
+      <c r="N25" t="s">
+        <v>266</v>
+      </c>
+      <c r="O25" t="s">
+        <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:15">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -6308,10 +8021,10 @@
         <v>91530</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F26">
         <v>91530</v>
@@ -6320,19 +8033,31 @@
         <v>93936</v>
       </c>
       <c r="H26" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I26" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="J26" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="K26" t="s">
-        <v>244</v>
+        <v>248</v>
+      </c>
+      <c r="L26" t="s">
+        <v>266</v>
+      </c>
+      <c r="M26" t="s">
+        <v>267</v>
+      </c>
+      <c r="N26" t="s">
+        <v>266</v>
+      </c>
+      <c r="O26" t="s">
+        <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:15">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -6343,10 +8068,10 @@
         <v>93941</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F27">
         <v>93941</v>
@@ -6355,19 +8080,31 @@
         <v>96507</v>
       </c>
       <c r="H27" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I27" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="J27" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="K27" t="s">
-        <v>245</v>
+        <v>249</v>
+      </c>
+      <c r="L27" t="s">
+        <v>266</v>
+      </c>
+      <c r="M27" t="s">
+        <v>267</v>
+      </c>
+      <c r="N27" t="s">
+        <v>266</v>
+      </c>
+      <c r="O27" t="s">
+        <v>293</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:15">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -6378,10 +8115,10 @@
         <v>96512</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F28">
         <v>96512</v>
@@ -6390,19 +8127,31 @@
         <v>99941</v>
       </c>
       <c r="H28" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="I28" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="J28" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="K28" t="s">
-        <v>246</v>
+        <v>250</v>
+      </c>
+      <c r="L28" t="s">
+        <v>266</v>
+      </c>
+      <c r="M28" t="s">
+        <v>267</v>
+      </c>
+      <c r="N28" t="s">
+        <v>266</v>
+      </c>
+      <c r="O28" t="s">
+        <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:15">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -6413,10 +8162,10 @@
         <v>99946</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F29">
         <v>99946</v>
@@ -6425,19 +8174,31 @@
         <v>103270</v>
       </c>
       <c r="H29" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I29" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J29" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="K29" t="s">
-        <v>247</v>
+        <v>251</v>
+      </c>
+      <c r="L29" t="s">
+        <v>266</v>
+      </c>
+      <c r="M29" t="s">
+        <v>267</v>
+      </c>
+      <c r="N29" t="s">
+        <v>266</v>
+      </c>
+      <c r="O29" t="s">
+        <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:15">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -6448,10 +8209,10 @@
         <v>103275</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F30">
         <v>103275</v>
@@ -6460,19 +8221,31 @@
         <v>106159</v>
       </c>
       <c r="H30" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I30" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="J30" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="K30" t="s">
-        <v>248</v>
+        <v>252</v>
+      </c>
+      <c r="L30" t="s">
+        <v>266</v>
+      </c>
+      <c r="M30" t="s">
+        <v>267</v>
+      </c>
+      <c r="N30" t="s">
+        <v>266</v>
+      </c>
+      <c r="O30" t="s">
+        <v>296</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:15">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -6483,10 +8256,10 @@
         <v>106164</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F31">
         <v>106164</v>
@@ -6495,19 +8268,31 @@
         <v>107763</v>
       </c>
       <c r="H31" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="I31" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J31" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K31" t="s">
-        <v>249</v>
+        <v>253</v>
+      </c>
+      <c r="L31" t="s">
+        <v>266</v>
+      </c>
+      <c r="M31" t="s">
+        <v>267</v>
+      </c>
+      <c r="N31" t="s">
+        <v>266</v>
+      </c>
+      <c r="O31" t="s">
+        <v>297</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:15">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -6518,10 +8303,10 @@
         <v>107768</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F32">
         <v>107768</v>
@@ -6530,19 +8315,31 @@
         <v>117718</v>
       </c>
       <c r="H32" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I32" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="J32" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="K32" t="s">
-        <v>250</v>
+        <v>254</v>
+      </c>
+      <c r="L32" t="s">
+        <v>266</v>
+      </c>
+      <c r="M32" t="s">
+        <v>267</v>
+      </c>
+      <c r="N32" t="s">
+        <v>266</v>
+      </c>
+      <c r="O32" t="s">
+        <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:15">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -6553,10 +8350,10 @@
         <v>117724</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F33">
         <v>117724</v>
@@ -6565,19 +8362,31 @@
         <v>119181</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I33" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="J33" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="K33" t="s">
-        <v>251</v>
+        <v>255</v>
+      </c>
+      <c r="L33" t="s">
+        <v>266</v>
+      </c>
+      <c r="M33" t="s">
+        <v>267</v>
+      </c>
+      <c r="N33" t="s">
+        <v>266</v>
+      </c>
+      <c r="O33" t="s">
+        <v>299</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:15">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -6588,10 +8397,10 @@
         <v>119187</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F34">
         <v>119187</v>
@@ -6600,19 +8409,31 @@
         <v>126276</v>
       </c>
       <c r="H34" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I34" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J34" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="K34" t="s">
-        <v>252</v>
+        <v>256</v>
+      </c>
+      <c r="L34" t="s">
+        <v>266</v>
+      </c>
+      <c r="M34" t="s">
+        <v>267</v>
+      </c>
+      <c r="N34" t="s">
+        <v>266</v>
+      </c>
+      <c r="O34" t="s">
+        <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:15">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -6623,10 +8444,10 @@
         <v>126282</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F35">
         <v>126282</v>
@@ -6635,19 +8456,31 @@
         <v>128737</v>
       </c>
       <c r="H35" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="I35" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J35" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="K35" t="s">
-        <v>253</v>
+        <v>257</v>
+      </c>
+      <c r="L35" t="s">
+        <v>266</v>
+      </c>
+      <c r="M35" t="s">
+        <v>267</v>
+      </c>
+      <c r="N35" t="s">
+        <v>266</v>
+      </c>
+      <c r="O35" t="s">
+        <v>301</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:15">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -6658,10 +8491,10 @@
         <v>128743</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F36">
         <v>128743</v>
@@ -6670,19 +8503,31 @@
         <v>129760</v>
       </c>
       <c r="H36" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="I36" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="J36" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K36" t="s">
-        <v>254</v>
+        <v>258</v>
+      </c>
+      <c r="L36" t="s">
+        <v>266</v>
+      </c>
+      <c r="M36" t="s">
+        <v>267</v>
+      </c>
+      <c r="N36" t="s">
+        <v>266</v>
+      </c>
+      <c r="O36" t="s">
+        <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:15">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -6693,10 +8538,10 @@
         <v>129766</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F37">
         <v>129766</v>
@@ -6705,19 +8550,31 @@
         <v>134094</v>
       </c>
       <c r="H37" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="I37" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="J37" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="K37" t="s">
-        <v>255</v>
+        <v>259</v>
+      </c>
+      <c r="L37" t="s">
+        <v>266</v>
+      </c>
+      <c r="M37" t="s">
+        <v>267</v>
+      </c>
+      <c r="N37" t="s">
+        <v>266</v>
+      </c>
+      <c r="O37" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:15">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -6728,10 +8585,10 @@
         <v>134100</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F38">
         <v>134100</v>
@@ -6740,19 +8597,31 @@
         <v>136241</v>
       </c>
       <c r="H38" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I38" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="J38" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="K38" t="s">
-        <v>256</v>
+        <v>260</v>
+      </c>
+      <c r="L38" t="s">
+        <v>266</v>
+      </c>
+      <c r="M38" t="s">
+        <v>267</v>
+      </c>
+      <c r="N38" t="s">
+        <v>266</v>
+      </c>
+      <c r="O38" t="s">
+        <v>304</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:15">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -6763,10 +8632,10 @@
         <v>136247</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F39">
         <v>136247</v>
@@ -6775,19 +8644,31 @@
         <v>137370</v>
       </c>
       <c r="H39" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="I39" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="J39" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K39" t="s">
-        <v>257</v>
+        <v>261</v>
+      </c>
+      <c r="L39" t="s">
+        <v>266</v>
+      </c>
+      <c r="M39" t="s">
+        <v>267</v>
+      </c>
+      <c r="N39" t="s">
+        <v>266</v>
+      </c>
+      <c r="O39" t="s">
+        <v>305</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:15">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -6798,10 +8679,10 @@
         <v>137376</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F40">
         <v>137376</v>
@@ -6810,19 +8691,31 @@
         <v>139709</v>
       </c>
       <c r="H40" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="I40" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="J40" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="K40" t="s">
-        <v>258</v>
+        <v>262</v>
+      </c>
+      <c r="L40" t="s">
+        <v>266</v>
+      </c>
+      <c r="M40" t="s">
+        <v>267</v>
+      </c>
+      <c r="N40" t="s">
+        <v>266</v>
+      </c>
+      <c r="O40" t="s">
+        <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:15">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -6833,10 +8726,10 @@
         <v>139715</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F41">
         <v>139715</v>
@@ -6845,19 +8738,31 @@
         <v>144325</v>
       </c>
       <c r="H41" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I41" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="J41" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="K41" t="s">
-        <v>259</v>
+        <v>263</v>
+      </c>
+      <c r="L41" t="s">
+        <v>266</v>
+      </c>
+      <c r="M41" t="s">
+        <v>267</v>
+      </c>
+      <c r="N41" t="s">
+        <v>266</v>
+      </c>
+      <c r="O41" t="s">
+        <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:15">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -6868,10 +8773,10 @@
         <v>144331</v>
       </c>
       <c r="D42" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F42">
         <v>144331</v>
@@ -6880,19 +8785,31 @@
         <v>146369</v>
       </c>
       <c r="H42" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="I42" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="J42" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="K42" t="s">
-        <v>260</v>
+        <v>264</v>
+      </c>
+      <c r="L42" t="s">
+        <v>266</v>
+      </c>
+      <c r="M42" t="s">
+        <v>267</v>
+      </c>
+      <c r="N42" t="s">
+        <v>266</v>
+      </c>
+      <c r="O42" t="s">
+        <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:15">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -6903,10 +8820,10 @@
         <v>146375</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F43">
         <v>146375</v>
@@ -6915,16 +8832,28 @@
         <v>148914</v>
       </c>
       <c r="H43" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I43" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="J43" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="K43" t="s">
-        <v>261</v>
+        <v>265</v>
+      </c>
+      <c r="L43" t="s">
+        <v>266</v>
+      </c>
+      <c r="M43" t="s">
+        <v>267</v>
+      </c>
+      <c r="N43" t="s">
+        <v>266</v>
+      </c>
+      <c r="O43" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>